<commit_message>
Updating the list for release 1.2.6 (2018_R2)
</commit_message>
<xml_diff>
--- a/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
+++ b/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSajikum\Documents\Linduino-git\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSajikum\Documents\ForRelease\Linduino\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="180000" windowHeight="40500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="450000" windowHeight="101250" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="901">
   <si>
     <t>Description</t>
   </si>
@@ -2714,6 +2714,15 @@
   </si>
   <si>
     <t>DC2365AC</t>
+  </si>
+  <si>
+    <t>LTC5556</t>
+  </si>
+  <si>
+    <t>Dual Programmable Downconverting Mixer with IF DVGAs</t>
+  </si>
+  <si>
+    <t>DC2693A</t>
   </si>
 </sst>
 </file>
@@ -3202,10 +3211,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:K287" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
-  <autoFilter ref="A3:K287"/>
-  <sortState ref="A4:K287">
-    <sortCondition ref="A3:A287"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:K288" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
+  <autoFilter ref="A3:K288"/>
+  <sortState ref="A4:K288">
+    <sortCondition ref="A3:A288"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="Product" dataDxfId="10" dataCellStyle="Normal"/>
@@ -3560,10 +3569,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L287"/>
+  <dimension ref="A1:L288"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="D242" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J257" sqref="J257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3588,8 +3597,8 @@
         <v>518</v>
       </c>
       <c r="E1" s="15">
-        <f>(COUNTIF(I4:I287,"Done")/(COUNTA(A4:A287)-COUNTIF(H4:H287,"No")))</f>
-        <v>0.8614718614718615</v>
+        <f>(COUNTIF(I4:I288,"Done")/(COUNTA(A4:A288)-COUNTIF(H4:H288,"No")))</f>
+        <v>0.86266094420600858</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3597,8 +3606,8 @@
         <v>519</v>
       </c>
       <c r="E2" s="8">
-        <f>(COUNTIF(F4:F287,"Yes")+(COUNTIF(F4:F287,"General"))+(COUNTIF(F4:F287,"Family")))/(COUNTA(A4:A287)-COUNTIF(H4:H287,"No"))</f>
-        <v>0.96536796536796532</v>
+        <f>(COUNTIF(F4:F288,"Yes")+(COUNTIF(F4:F288,"General"))+(COUNTIF(F4:F288,"Family")))/(COUNTA(A4:A288)-COUNTIF(H4:H288,"No"))</f>
+        <v>0.96566523605150212</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -10721,174 +10730,182 @@
       <c r="K256" s="25"/>
     </row>
     <row r="257" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A257" s="25" t="s">
-        <v>688</v>
-      </c>
-      <c r="B257" s="25" t="s">
+      <c r="A257" s="13" t="s">
+        <v>898</v>
+      </c>
+      <c r="B257" s="13" t="s">
         <v>861</v>
       </c>
-      <c r="C257" s="25" t="s">
-        <v>691</v>
-      </c>
-      <c r="D257" s="25" t="s">
-        <v>722</v>
-      </c>
-      <c r="E257" s="25" t="s">
-        <v>692</v>
-      </c>
-      <c r="F257" s="26" t="s">
-        <v>497</v>
-      </c>
-      <c r="G257" s="26"/>
-      <c r="H257" s="26"/>
-      <c r="I257" s="26" t="s">
-        <v>517</v>
-      </c>
-      <c r="J257" s="26" t="s">
+      <c r="C257" s="16" t="s">
+        <v>899</v>
+      </c>
+      <c r="D257" s="29"/>
+      <c r="E257" s="13" t="s">
+        <v>900</v>
+      </c>
+      <c r="F257" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G257" s="29"/>
+      <c r="H257" s="29"/>
+      <c r="I257" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J257" s="13" t="s">
         <v>732</v>
       </c>
-      <c r="K257" s="25"/>
+      <c r="K257" s="29"/>
     </row>
     <row r="258" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A258" s="25" t="s">
-        <v>544</v>
+        <v>688</v>
       </c>
       <c r="B258" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C258" s="25" t="s">
-        <v>546</v>
+        <v>691</v>
       </c>
       <c r="D258" s="25" t="s">
         <v>722</v>
       </c>
       <c r="E258" s="25" t="s">
-        <v>545</v>
-      </c>
-      <c r="F258" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G258" s="25"/>
-      <c r="H258" s="25"/>
-      <c r="I258" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J258" s="25" t="s">
-        <v>523</v>
+        <v>692</v>
+      </c>
+      <c r="F258" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="G258" s="26"/>
+      <c r="H258" s="26"/>
+      <c r="I258" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="J258" s="26" t="s">
+        <v>732</v>
       </c>
       <c r="K258" s="25"/>
     </row>
     <row r="259" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A259" s="25" t="s">
-        <v>598</v>
-      </c>
-      <c r="B259" s="25"/>
+        <v>544</v>
+      </c>
+      <c r="B259" s="25" t="s">
+        <v>861</v>
+      </c>
       <c r="C259" s="25" t="s">
-        <v>599</v>
-      </c>
-      <c r="D259" s="25"/>
+        <v>546</v>
+      </c>
+      <c r="D259" s="25" t="s">
+        <v>722</v>
+      </c>
       <c r="E259" s="25" t="s">
-        <v>202</v>
+        <v>545</v>
       </c>
       <c r="F259" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G259" s="25"/>
-      <c r="H259" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="I259" s="25"/>
+      <c r="H259" s="25"/>
+      <c r="I259" s="25" t="s">
+        <v>517</v>
+      </c>
       <c r="J259" s="25" t="s">
-        <v>596</v>
+        <v>523</v>
       </c>
       <c r="K259" s="25"/>
     </row>
     <row r="260" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A260" s="25" t="s">
-        <v>526</v>
-      </c>
-      <c r="B260" s="25" t="s">
-        <v>861</v>
-      </c>
+        <v>598</v>
+      </c>
+      <c r="B260" s="25"/>
       <c r="C260" s="25" t="s">
-        <v>646</v>
-      </c>
-      <c r="D260" s="25" t="s">
-        <v>722</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="D260" s="25"/>
       <c r="E260" s="25" t="s">
-        <v>648</v>
-      </c>
-      <c r="F260" s="26" t="s">
-        <v>497</v>
-      </c>
-      <c r="G260" s="26"/>
-      <c r="H260" s="26"/>
-      <c r="I260" s="26" t="s">
-        <v>517</v>
-      </c>
-      <c r="J260" s="26" t="s">
-        <v>641</v>
+        <v>202</v>
+      </c>
+      <c r="F260" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="G260" s="25"/>
+      <c r="H260" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="I260" s="25"/>
+      <c r="J260" s="25" t="s">
+        <v>596</v>
       </c>
       <c r="K260" s="25"/>
     </row>
     <row r="261" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A261" s="25" t="s">
-        <v>642</v>
-      </c>
-      <c r="B261" s="25"/>
+        <v>526</v>
+      </c>
+      <c r="B261" s="25" t="s">
+        <v>861</v>
+      </c>
       <c r="C261" s="25" t="s">
-        <v>647</v>
-      </c>
-      <c r="D261" s="25"/>
+        <v>646</v>
+      </c>
+      <c r="D261" s="25" t="s">
+        <v>722</v>
+      </c>
       <c r="E261" s="25" t="s">
-        <v>649</v>
-      </c>
-      <c r="F261" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="G261" s="25"/>
-      <c r="H261" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="I261" s="25"/>
-      <c r="J261" s="25"/>
+        <v>648</v>
+      </c>
+      <c r="F261" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="G261" s="26"/>
+      <c r="H261" s="26"/>
+      <c r="I261" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="J261" s="26" t="s">
+        <v>641</v>
+      </c>
       <c r="K261" s="25"/>
     </row>
     <row r="262" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A262" s="25" t="s">
-        <v>211</v>
+        <v>642</v>
       </c>
       <c r="B262" s="25"/>
       <c r="C262" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="D262" s="25"/>
+        <v>647</v>
+      </c>
+      <c r="D262" s="25" t="s">
+        <v>722</v>
+      </c>
       <c r="E262" s="25" t="s">
-        <v>209</v>
+        <v>649</v>
       </c>
       <c r="F262" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G262" s="25"/>
-      <c r="H262" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="I262" s="25"/>
-      <c r="J262" s="25"/>
+      <c r="H262" s="25"/>
+      <c r="I262" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J262" s="25" t="s">
+        <v>641</v>
+      </c>
       <c r="K262" s="25"/>
     </row>
     <row r="263" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A263" s="25" t="s">
-        <v>343</v>
+        <v>211</v>
       </c>
       <c r="B263" s="25"/>
       <c r="C263" s="25" t="s">
-        <v>342</v>
+        <v>210</v>
       </c>
       <c r="D263" s="25"/>
       <c r="E263" s="25" t="s">
-        <v>341</v>
+        <v>209</v>
       </c>
       <c r="F263" s="25" t="s">
         <v>498</v>
@@ -10903,44 +10920,40 @@
     </row>
     <row r="264" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A264" s="25" t="s">
-        <v>621</v>
-      </c>
-      <c r="B264" s="25" t="s">
-        <v>862</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="B264" s="25"/>
       <c r="C264" s="25" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="D264" s="25"/>
       <c r="E264" s="25" t="s">
-        <v>190</v>
+        <v>341</v>
       </c>
       <c r="F264" s="25" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G264" s="25"/>
-      <c r="H264" s="25"/>
-      <c r="I264" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J264" s="25" t="s">
-        <v>620</v>
-      </c>
+      <c r="H264" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="I264" s="25"/>
+      <c r="J264" s="25"/>
       <c r="K264" s="25"/>
     </row>
     <row r="265" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A265" s="25" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B265" s="25" t="s">
         <v>862</v>
       </c>
       <c r="C265" s="25" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D265" s="25"/>
       <c r="E265" s="25" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="F265" s="25" t="s">
         <v>497</v>
@@ -10957,38 +10970,42 @@
     </row>
     <row r="266" spans="1:12" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A266" s="25" t="s">
-        <v>623</v>
-      </c>
-      <c r="B266" s="25"/>
+        <v>622</v>
+      </c>
+      <c r="B266" s="25" t="s">
+        <v>862</v>
+      </c>
       <c r="C266" s="25" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D266" s="25"/>
       <c r="E266" s="25" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F266" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G266" s="25"/>
-      <c r="H266" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="I266" s="25"/>
-      <c r="J266" s="25"/>
+      <c r="H266" s="25"/>
+      <c r="I266" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J266" s="25" t="s">
+        <v>620</v>
+      </c>
       <c r="K266" s="25"/>
     </row>
     <row r="267" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A267" s="25" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B267" s="25"/>
       <c r="C267" s="25" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="D267" s="25"/>
       <c r="E267" s="25" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="F267" s="25" t="s">
         <v>498</v>
@@ -11003,44 +11020,40 @@
     </row>
     <row r="268" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A268" s="25" t="s">
-        <v>503</v>
-      </c>
-      <c r="B268" s="25" t="s">
-        <v>862</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="B268" s="25"/>
       <c r="C268" s="25" t="s">
-        <v>502</v>
+        <v>100</v>
       </c>
       <c r="D268" s="25"/>
       <c r="E268" s="25" t="s">
-        <v>501</v>
+        <v>99</v>
       </c>
       <c r="F268" s="25" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G268" s="25"/>
-      <c r="H268" s="25"/>
-      <c r="I268" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J268" s="25" t="s">
-        <v>620</v>
-      </c>
+      <c r="H268" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="I268" s="25"/>
+      <c r="J268" s="25"/>
       <c r="K268" s="25"/>
     </row>
     <row r="269" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A269" s="25" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B269" s="25" t="s">
         <v>862</v>
       </c>
       <c r="C269" s="25" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D269" s="25"/>
       <c r="E269" s="25" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F269" s="25" t="s">
         <v>497</v>
@@ -11057,17 +11070,17 @@
     </row>
     <row r="270" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A270" s="25" t="s">
-        <v>804</v>
+        <v>506</v>
       </c>
       <c r="B270" s="25" t="s">
         <v>862</v>
       </c>
       <c r="C270" s="25" t="s">
-        <v>805</v>
+        <v>505</v>
       </c>
       <c r="D270" s="25"/>
       <c r="E270" s="25" t="s">
-        <v>806</v>
+        <v>504</v>
       </c>
       <c r="F270" s="25" t="s">
         <v>497</v>
@@ -11084,72 +11097,70 @@
     </row>
     <row r="271" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A271" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B271" s="25"/>
+        <v>804</v>
+      </c>
+      <c r="B271" s="25" t="s">
+        <v>862</v>
+      </c>
       <c r="C271" s="25" t="s">
-        <v>24</v>
+        <v>805</v>
       </c>
       <c r="D271" s="25"/>
       <c r="E271" s="25" t="s">
-        <v>23</v>
+        <v>806</v>
       </c>
       <c r="F271" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G271" s="25"/>
-      <c r="H271" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="I271" s="25"/>
-      <c r="J271" s="25"/>
+      <c r="H271" s="25"/>
+      <c r="I271" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J271" s="25" t="s">
+        <v>620</v>
+      </c>
       <c r="K271" s="25"/>
     </row>
     <row r="272" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A272" s="25" t="s">
-        <v>509</v>
-      </c>
-      <c r="B272" s="25" t="s">
-        <v>861</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B272" s="25"/>
       <c r="C272" s="25" t="s">
-        <v>508</v>
-      </c>
-      <c r="D272" s="25" t="s">
-        <v>722</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D272" s="25"/>
       <c r="E272" s="25" t="s">
-        <v>811</v>
-      </c>
-      <c r="F272" s="26" t="s">
-        <v>497</v>
-      </c>
-      <c r="G272" s="26"/>
-      <c r="H272" s="26"/>
-      <c r="I272" s="26" t="s">
-        <v>517</v>
-      </c>
-      <c r="J272" s="26" t="s">
-        <v>551</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F272" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="G272" s="25"/>
+      <c r="H272" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="I272" s="25"/>
+      <c r="J272" s="25"/>
       <c r="K272" s="25"/>
       <c r="L272" s="20"/>
     </row>
     <row r="273" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A273" s="25" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B273" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C273" s="25" t="s">
-        <v>812</v>
+        <v>508</v>
       </c>
       <c r="D273" s="25" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E273" s="25" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F273" s="26" t="s">
         <v>497</v>
@@ -11166,48 +11177,48 @@
     </row>
     <row r="274" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A274" s="25" t="s">
-        <v>106</v>
+        <v>507</v>
       </c>
       <c r="B274" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C274" s="25" t="s">
-        <v>105</v>
+        <v>812</v>
       </c>
       <c r="D274" s="25" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="E274" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F274" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G274" s="25"/>
-      <c r="H274" s="25"/>
-      <c r="I274" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J274" s="25" t="s">
-        <v>549</v>
+        <v>813</v>
+      </c>
+      <c r="F274" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="G274" s="26"/>
+      <c r="H274" s="26"/>
+      <c r="I274" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="J274" s="26" t="s">
+        <v>551</v>
       </c>
       <c r="K274" s="25"/>
     </row>
     <row r="275" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A275" s="25" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="B275" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C275" s="25" t="s">
-        <v>617</v>
+        <v>105</v>
       </c>
       <c r="D275" s="25" t="s">
         <v>722</v>
       </c>
       <c r="E275" s="25" t="s">
-        <v>618</v>
+        <v>104</v>
       </c>
       <c r="F275" s="25" t="s">
         <v>497</v>
@@ -11220,25 +11231,23 @@
       <c r="J275" s="25" t="s">
         <v>549</v>
       </c>
-      <c r="K275" s="25" t="s">
-        <v>490</v>
-      </c>
+      <c r="K275" s="25"/>
     </row>
     <row r="276" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A276" s="25" t="s">
-        <v>570</v>
+        <v>38</v>
       </c>
       <c r="B276" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C276" s="25" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D276" s="25" t="s">
         <v>722</v>
       </c>
       <c r="E276" s="25" t="s">
-        <v>571</v>
+        <v>618</v>
       </c>
       <c r="F276" s="25" t="s">
         <v>497</v>
@@ -11251,23 +11260,25 @@
       <c r="J276" s="25" t="s">
         <v>549</v>
       </c>
-      <c r="K276" s="25"/>
+      <c r="K276" s="25" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="277" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A277" s="25" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B277" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C277" s="25" t="s">
-        <v>697</v>
+        <v>615</v>
       </c>
       <c r="D277" s="25" t="s">
         <v>722</v>
       </c>
       <c r="E277" s="25" t="s">
-        <v>698</v>
+        <v>571</v>
       </c>
       <c r="F277" s="25" t="s">
         <v>497</v>
@@ -11284,19 +11295,19 @@
     </row>
     <row r="278" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A278" s="25" t="s">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="B278" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C278" s="25" t="s">
-        <v>616</v>
+        <v>697</v>
       </c>
       <c r="D278" s="25" t="s">
         <v>722</v>
       </c>
       <c r="E278" s="25" t="s">
-        <v>548</v>
+        <v>698</v>
       </c>
       <c r="F278" s="25" t="s">
         <v>497</v>
@@ -11313,19 +11324,19 @@
     </row>
     <row r="279" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A279" s="25" t="s">
-        <v>578</v>
+        <v>547</v>
       </c>
       <c r="B279" s="25" t="s">
         <v>861</v>
       </c>
       <c r="C279" s="25" t="s">
-        <v>662</v>
+        <v>616</v>
       </c>
       <c r="D279" s="25" t="s">
         <v>722</v>
       </c>
       <c r="E279" s="25" t="s">
-        <v>725</v>
+        <v>548</v>
       </c>
       <c r="F279" s="25" t="s">
         <v>497</v>
@@ -11341,33 +11352,37 @@
       <c r="K279" s="25"/>
     </row>
     <row r="280" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A280" s="13" t="s">
-        <v>868</v>
+      <c r="A280" s="25" t="s">
+        <v>578</v>
       </c>
       <c r="B280" s="25" t="s">
         <v>861</v>
       </c>
-      <c r="C280" s="29"/>
-      <c r="D280" s="29"/>
-      <c r="E280" s="13" t="s">
-        <v>870</v>
+      <c r="C280" s="25" t="s">
+        <v>662</v>
+      </c>
+      <c r="D280" s="25" t="s">
+        <v>722</v>
+      </c>
+      <c r="E280" s="25" t="s">
+        <v>725</v>
       </c>
       <c r="F280" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="G280" s="29"/>
-      <c r="H280" s="29"/>
+      <c r="G280" s="25"/>
+      <c r="H280" s="25"/>
       <c r="I280" s="25" t="s">
         <v>517</v>
       </c>
       <c r="J280" s="25" t="s">
         <v>549</v>
       </c>
-      <c r="K280" s="29"/>
+      <c r="K280" s="25"/>
     </row>
     <row r="281" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A281" s="13" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B281" s="25" t="s">
         <v>861</v>
@@ -11375,7 +11390,7 @@
       <c r="C281" s="29"/>
       <c r="D281" s="29"/>
       <c r="E281" s="13" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F281" s="25" t="s">
         <v>497</v>
@@ -11391,115 +11406,111 @@
       <c r="K281" s="29"/>
     </row>
     <row r="282" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A282" s="25" t="s">
-        <v>575</v>
+      <c r="A282" s="13" t="s">
+        <v>869</v>
       </c>
       <c r="B282" s="25" t="s">
         <v>861</v>
       </c>
-      <c r="C282" s="25" t="s">
-        <v>619</v>
-      </c>
-      <c r="D282" s="25" t="s">
-        <v>722</v>
-      </c>
-      <c r="E282" s="25" t="s">
-        <v>576</v>
+      <c r="C282" s="29"/>
+      <c r="D282" s="29"/>
+      <c r="E282" s="13" t="s">
+        <v>871</v>
       </c>
       <c r="F282" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="G282" s="25"/>
-      <c r="H282" s="25"/>
+      <c r="G282" s="29"/>
+      <c r="H282" s="29"/>
       <c r="I282" s="25" t="s">
         <v>517</v>
       </c>
       <c r="J282" s="25" t="s">
         <v>549</v>
       </c>
-      <c r="K282" s="25"/>
+      <c r="K282" s="29"/>
     </row>
     <row r="283" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A283" s="13" t="s">
-        <v>716</v>
-      </c>
-      <c r="B283" s="13" t="s">
-        <v>847</v>
-      </c>
-      <c r="C283" s="13" t="s">
-        <v>717</v>
-      </c>
-      <c r="D283" s="13"/>
-      <c r="E283" s="13" t="s">
-        <v>718</v>
-      </c>
-      <c r="F283" s="14" t="s">
-        <v>497</v>
-      </c>
-      <c r="G283" s="14"/>
-      <c r="H283" s="14"/>
-      <c r="I283" s="14" t="s">
-        <v>517</v>
-      </c>
-      <c r="J283" s="14" t="s">
-        <v>752</v>
-      </c>
-      <c r="K283" s="13"/>
+      <c r="A283" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="B283" s="25" t="s">
+        <v>861</v>
+      </c>
+      <c r="C283" s="25" t="s">
+        <v>619</v>
+      </c>
+      <c r="D283" s="25" t="s">
+        <v>722</v>
+      </c>
+      <c r="E283" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="F283" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="G283" s="25"/>
+      <c r="H283" s="25"/>
+      <c r="I283" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J283" s="25" t="s">
+        <v>549</v>
+      </c>
+      <c r="K283" s="25"/>
     </row>
     <row r="284" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A284" s="13" t="s">
-        <v>673</v>
+        <v>716</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>856</v>
-      </c>
-      <c r="C284" s="21" t="s">
-        <v>675</v>
-      </c>
-      <c r="D284" s="21" t="s">
-        <v>740</v>
-      </c>
+        <v>847</v>
+      </c>
+      <c r="C284" s="13" t="s">
+        <v>717</v>
+      </c>
+      <c r="D284" s="13"/>
       <c r="E284" s="13" t="s">
-        <v>803</v>
-      </c>
-      <c r="F284" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G284" s="13"/>
-      <c r="H284" s="13"/>
-      <c r="I284" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J284" s="13" t="s">
-        <v>543</v>
+        <v>718</v>
+      </c>
+      <c r="F284" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="G284" s="14"/>
+      <c r="H284" s="14"/>
+      <c r="I284" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="J284" s="14" t="s">
+        <v>752</v>
       </c>
       <c r="K284" s="13"/>
     </row>
     <row r="285" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A285" s="13" t="s">
-        <v>742</v>
+        <v>673</v>
       </c>
       <c r="B285" s="13" t="s">
         <v>856</v>
       </c>
       <c r="C285" s="21" t="s">
-        <v>743</v>
-      </c>
-      <c r="D285" s="13" t="s">
+        <v>675</v>
+      </c>
+      <c r="D285" s="21" t="s">
         <v>740</v>
       </c>
       <c r="E285" s="13" t="s">
-        <v>744</v>
-      </c>
-      <c r="F285" s="14" t="s">
-        <v>497</v>
-      </c>
-      <c r="G285" s="14"/>
-      <c r="H285" s="14"/>
-      <c r="I285" s="14" t="s">
-        <v>517</v>
-      </c>
-      <c r="J285" s="14" t="s">
+        <v>803</v>
+      </c>
+      <c r="F285" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G285" s="13"/>
+      <c r="H285" s="13"/>
+      <c r="I285" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J285" s="13" t="s">
         <v>543</v>
       </c>
       <c r="K285" s="13"/>
@@ -11511,43 +11522,43 @@
       <c r="B286" s="13" t="s">
         <v>856</v>
       </c>
-      <c r="C286" s="13" t="s">
+      <c r="C286" s="21" t="s">
         <v>743</v>
       </c>
       <c r="D286" s="13" t="s">
         <v>740</v>
       </c>
       <c r="E286" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="F286" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G286" s="13"/>
-      <c r="H286" s="13"/>
-      <c r="I286" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J286" s="13" t="s">
+        <v>744</v>
+      </c>
+      <c r="F286" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="G286" s="14"/>
+      <c r="H286" s="14"/>
+      <c r="I286" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="J286" s="14" t="s">
         <v>543</v>
       </c>
       <c r="K286" s="13"/>
     </row>
     <row r="287" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A287" s="13" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>848</v>
+        <v>856</v>
       </c>
       <c r="C287" s="13" t="s">
-        <v>758</v>
+        <v>743</v>
       </c>
       <c r="D287" s="13" t="s">
-        <v>723</v>
+        <v>740</v>
       </c>
       <c r="E287" s="13" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="F287" s="13" t="s">
         <v>497</v>
@@ -11558,13 +11569,42 @@
         <v>517</v>
       </c>
       <c r="J287" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="K287" s="13"/>
+    </row>
+    <row r="288" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A288" s="13" t="s">
+        <v>757</v>
+      </c>
+      <c r="B288" s="13" t="s">
+        <v>848</v>
+      </c>
+      <c r="C288" s="13" t="s">
+        <v>758</v>
+      </c>
+      <c r="D288" s="13" t="s">
+        <v>723</v>
+      </c>
+      <c r="E288" s="13" t="s">
+        <v>759</v>
+      </c>
+      <c r="F288" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G288" s="13"/>
+      <c r="H288" s="13"/>
+      <c r="I288" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J288" s="13" t="s">
         <v>611</v>
       </c>
-      <c r="K287" s="13"/>
+      <c r="K288" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A1:G407">
-    <sortCondition ref="A1:A407"/>
+  <sortState ref="A1:G408">
+    <sortCondition ref="A1:A408"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Contact Cuyler Latorraca or Jothish Joseph Kalathil for questions. Adding support for LTC6810, LTC6812, LTC6813.
LTC681x file changes
Added functions for commands wrsctrl, rdsctrl, stsctrl and  axow.
Added LTC681x_run_gpio_openwire()  and LTC681x_run_openwire_multi()
Changed LTC681x_run_cell_adc_st()
Changed cell_asic structure to compatible with LTC6810

LTC 6811 file changes
Added functions for commands wrsctrl, rdsctrl and stsctrl
Added  LTC681x_run_openwire_multi()

DC2259.ino changes
Bug fix in LTC6811_run_cell_adc_st()
Added all the missing commands
</commit_message>
<xml_diff>
--- a/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
+++ b/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSajikum\Documents\Linduino\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C22D943-B400-411B-927A-E9B1647D2F8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0C9D5-BB0B-4981-9CE1-0AFFD1B65E99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="436900" windowHeight="101253" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="913">
   <si>
     <t>Description</t>
   </si>
@@ -2746,6 +2746,27 @@
   </si>
   <si>
     <t>Catherine Chang</t>
+  </si>
+  <si>
+    <t>LTC6810</t>
+  </si>
+  <si>
+    <t>LTC6812</t>
+  </si>
+  <si>
+    <t>LTC6813</t>
+  </si>
+  <si>
+    <t>DC2515</t>
+  </si>
+  <si>
+    <t>DC2350AA</t>
+  </si>
+  <si>
+    <t>DC2350AB</t>
+  </si>
+  <si>
+    <t>Jothish Joseph Kalathil</t>
   </si>
 </sst>
 </file>
@@ -3231,10 +3252,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A3:K289" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
-  <autoFilter ref="A3:K289" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState ref="A4:K288">
-    <sortCondition ref="A3:A288"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A3:K292" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
+  <autoFilter ref="A3:K292" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState ref="A4:K291">
+    <sortCondition ref="A3:A291"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Product" dataDxfId="10" dataCellStyle="Normal"/>
@@ -3589,10 +3610,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L289"/>
+  <dimension ref="A1:L292"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A265" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J289" sqref="J289"/>
+      <selection activeCell="J271" sqref="J271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -3617,8 +3638,8 @@
         <v>518</v>
       </c>
       <c r="E1" s="14">
-        <f>(COUNTIF(I4:I289,"Done")/(COUNTA(A4:A289)-COUNTIF(H4:H289,"No")))</f>
-        <v>0.86324786324786329</v>
+        <f>(COUNTIF(I4:I292,"Done")/(COUNTA(A4:A292)-COUNTIF(H4:H292,"No")))</f>
+        <v>0.86497890295358648</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
@@ -3626,8 +3647,8 @@
         <v>519</v>
       </c>
       <c r="E2" s="14">
-        <f>(COUNTIF(F4:F289,"Yes")+(COUNTIF(F4:F289,"General"))+(COUNTIF(F4:F289,"Family")))/(COUNTA(A4:A289)-COUNTIF(H4:H289,"No"))</f>
-        <v>0.96581196581196582</v>
+        <f>(COUNTIF(F4:F292,"Yes")+(COUNTIF(F4:F292,"General"))+(COUNTIF(F4:F292,"Family")))/(COUNTA(A4:A292)-COUNTIF(H4:H292,"No"))</f>
+        <v>0.96624472573839659</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -11116,8 +11137,8 @@
       <c r="K270" s="24"/>
     </row>
     <row r="271" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A271" s="24" t="s">
-        <v>804</v>
+      <c r="A271" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="B271" s="24" t="s">
         <v>862</v>
@@ -11125,209 +11146,199 @@
       <c r="C271" s="24" t="s">
         <v>805</v>
       </c>
-      <c r="D271" s="24"/>
-      <c r="E271" s="24" t="s">
-        <v>806</v>
+      <c r="D271" s="28"/>
+      <c r="E271" s="12" t="s">
+        <v>909</v>
       </c>
       <c r="F271" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G271" s="24"/>
-      <c r="H271" s="24"/>
+      <c r="G271" s="28"/>
+      <c r="H271" s="28"/>
       <c r="I271" s="24" t="s">
         <v>517</v>
       </c>
-      <c r="J271" s="24" t="s">
-        <v>620</v>
-      </c>
-      <c r="K271" s="24"/>
+      <c r="J271" s="12" t="s">
+        <v>912</v>
+      </c>
+      <c r="K271" s="28"/>
     </row>
     <row r="272" spans="1:12" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B272" s="24"/>
+        <v>804</v>
+      </c>
+      <c r="B272" s="24" t="s">
+        <v>862</v>
+      </c>
       <c r="C272" s="24" t="s">
-        <v>24</v>
+        <v>805</v>
       </c>
       <c r="D272" s="24"/>
       <c r="E272" s="24" t="s">
-        <v>23</v>
+        <v>806</v>
       </c>
       <c r="F272" s="24" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G272" s="24"/>
-      <c r="H272" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I272" s="24"/>
-      <c r="J272" s="24"/>
+      <c r="H272" s="24"/>
+      <c r="I272" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J272" s="24" t="s">
+        <v>620</v>
+      </c>
       <c r="K272" s="24"/>
       <c r="L272" s="19"/>
     </row>
     <row r="273" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A273" s="24" t="s">
-        <v>509</v>
+      <c r="A273" s="12" t="s">
+        <v>907</v>
       </c>
       <c r="B273" s="24" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C273" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="D273" s="24" t="s">
-        <v>722</v>
-      </c>
-      <c r="E273" s="24" t="s">
-        <v>811</v>
-      </c>
-      <c r="F273" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G273" s="25"/>
-      <c r="H273" s="25"/>
-      <c r="I273" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J273" s="25" t="s">
-        <v>551</v>
-      </c>
-      <c r="K273" s="24"/>
+        <v>805</v>
+      </c>
+      <c r="D273" s="28"/>
+      <c r="E273" s="12" t="s">
+        <v>910</v>
+      </c>
+      <c r="F273" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G273" s="28"/>
+      <c r="H273" s="28"/>
+      <c r="I273" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J273" s="12" t="s">
+        <v>912</v>
+      </c>
+      <c r="K273" s="28"/>
     </row>
     <row r="274" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A274" s="24" t="s">
-        <v>507</v>
+      <c r="A274" s="12" t="s">
+        <v>908</v>
       </c>
       <c r="B274" s="24" t="s">
-        <v>861</v>
-      </c>
-      <c r="C274" s="24" t="s">
-        <v>812</v>
-      </c>
-      <c r="D274" s="24" t="s">
-        <v>723</v>
-      </c>
-      <c r="E274" s="24" t="s">
-        <v>813</v>
-      </c>
-      <c r="F274" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G274" s="25"/>
-      <c r="H274" s="25"/>
-      <c r="I274" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J274" s="25" t="s">
-        <v>551</v>
-      </c>
-      <c r="K274" s="24"/>
+        <v>862</v>
+      </c>
+      <c r="C274" s="28"/>
+      <c r="D274" s="28"/>
+      <c r="E274" s="12" t="s">
+        <v>911</v>
+      </c>
+      <c r="F274" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G274" s="28"/>
+      <c r="H274" s="28"/>
+      <c r="I274" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J274" s="12" t="s">
+        <v>912</v>
+      </c>
+      <c r="K274" s="28"/>
     </row>
     <row r="275" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B275" s="24" t="s">
-        <v>861</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B275" s="24"/>
       <c r="C275" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D275" s="24" t="s">
-        <v>722</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D275" s="24"/>
       <c r="E275" s="24" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="F275" s="24" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G275" s="24"/>
-      <c r="H275" s="24"/>
-      <c r="I275" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J275" s="24" t="s">
-        <v>549</v>
-      </c>
+      <c r="H275" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="I275" s="24"/>
+      <c r="J275" s="24"/>
       <c r="K275" s="24"/>
     </row>
     <row r="276" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="24" t="s">
-        <v>38</v>
+        <v>509</v>
       </c>
       <c r="B276" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C276" s="24" t="s">
-        <v>617</v>
+        <v>508</v>
       </c>
       <c r="D276" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E276" s="24" t="s">
-        <v>618</v>
-      </c>
-      <c r="F276" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="G276" s="24"/>
-      <c r="H276" s="24"/>
-      <c r="I276" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J276" s="24" t="s">
-        <v>549</v>
-      </c>
-      <c r="K276" s="24" t="s">
-        <v>490</v>
-      </c>
+        <v>811</v>
+      </c>
+      <c r="F276" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="G276" s="25"/>
+      <c r="H276" s="25"/>
+      <c r="I276" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J276" s="25" t="s">
+        <v>551</v>
+      </c>
+      <c r="K276" s="24"/>
     </row>
     <row r="277" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="24" t="s">
-        <v>570</v>
+        <v>507</v>
       </c>
       <c r="B277" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C277" s="24" t="s">
-        <v>615</v>
+        <v>812</v>
       </c>
       <c r="D277" s="24" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="E277" s="24" t="s">
-        <v>571</v>
-      </c>
-      <c r="F277" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="G277" s="24"/>
-      <c r="H277" s="24"/>
-      <c r="I277" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J277" s="24" t="s">
-        <v>549</v>
+        <v>813</v>
+      </c>
+      <c r="F277" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="G277" s="25"/>
+      <c r="H277" s="25"/>
+      <c r="I277" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J277" s="25" t="s">
+        <v>551</v>
       </c>
       <c r="K277" s="24"/>
     </row>
     <row r="278" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="24" t="s">
-        <v>569</v>
+        <v>106</v>
       </c>
       <c r="B278" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C278" s="24" t="s">
-        <v>697</v>
+        <v>105</v>
       </c>
       <c r="D278" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E278" s="24" t="s">
-        <v>698</v>
+        <v>104</v>
       </c>
       <c r="F278" s="24" t="s">
         <v>497</v>
@@ -11344,19 +11355,19 @@
     </row>
     <row r="279" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="24" t="s">
-        <v>547</v>
+        <v>38</v>
       </c>
       <c r="B279" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C279" s="24" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D279" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E279" s="24" t="s">
-        <v>548</v>
+        <v>618</v>
       </c>
       <c r="F279" s="24" t="s">
         <v>497</v>
@@ -11369,23 +11380,25 @@
       <c r="J279" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K279" s="24"/>
+      <c r="K279" s="24" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="280" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="24" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="B280" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C280" s="24" t="s">
-        <v>662</v>
+        <v>615</v>
       </c>
       <c r="D280" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E280" s="24" t="s">
-        <v>725</v>
+        <v>571</v>
       </c>
       <c r="F280" s="24" t="s">
         <v>497</v>
@@ -11401,70 +11414,78 @@
       <c r="K280" s="24"/>
     </row>
     <row r="281" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A281" s="12" t="s">
-        <v>868</v>
+      <c r="A281" s="24" t="s">
+        <v>569</v>
       </c>
       <c r="B281" s="24" t="s">
         <v>861</v>
       </c>
-      <c r="C281" s="28"/>
-      <c r="D281" s="28"/>
-      <c r="E281" s="12" t="s">
-        <v>870</v>
+      <c r="C281" s="24" t="s">
+        <v>697</v>
+      </c>
+      <c r="D281" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="E281" s="24" t="s">
+        <v>698</v>
       </c>
       <c r="F281" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G281" s="28"/>
-      <c r="H281" s="28"/>
+      <c r="G281" s="24"/>
+      <c r="H281" s="24"/>
       <c r="I281" s="24" t="s">
         <v>517</v>
       </c>
       <c r="J281" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K281" s="28"/>
+      <c r="K281" s="24"/>
     </row>
     <row r="282" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A282" s="12" t="s">
-        <v>869</v>
+      <c r="A282" s="24" t="s">
+        <v>547</v>
       </c>
       <c r="B282" s="24" t="s">
         <v>861</v>
       </c>
-      <c r="C282" s="28"/>
-      <c r="D282" s="28"/>
-      <c r="E282" s="12" t="s">
-        <v>871</v>
+      <c r="C282" s="24" t="s">
+        <v>616</v>
+      </c>
+      <c r="D282" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="E282" s="24" t="s">
+        <v>548</v>
       </c>
       <c r="F282" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G282" s="28"/>
-      <c r="H282" s="28"/>
+      <c r="G282" s="24"/>
+      <c r="H282" s="24"/>
       <c r="I282" s="24" t="s">
         <v>517</v>
       </c>
       <c r="J282" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K282" s="28"/>
+      <c r="K282" s="24"/>
     </row>
     <row r="283" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="24" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B283" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C283" s="24" t="s">
-        <v>619</v>
+        <v>662</v>
       </c>
       <c r="D283" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E283" s="24" t="s">
-        <v>576</v>
+        <v>725</v>
       </c>
       <c r="F283" s="24" t="s">
         <v>497</v>
@@ -11481,133 +11502,125 @@
     </row>
     <row r="284" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="12" t="s">
-        <v>716</v>
-      </c>
-      <c r="B284" s="12" t="s">
-        <v>847</v>
-      </c>
-      <c r="C284" s="12" t="s">
-        <v>717</v>
-      </c>
-      <c r="D284" s="12"/>
+        <v>868</v>
+      </c>
+      <c r="B284" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="C284" s="28"/>
+      <c r="D284" s="28"/>
       <c r="E284" s="12" t="s">
-        <v>718</v>
-      </c>
-      <c r="F284" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G284" s="13"/>
-      <c r="H284" s="13"/>
-      <c r="I284" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J284" s="13" t="s">
-        <v>752</v>
-      </c>
-      <c r="K284" s="12"/>
+        <v>870</v>
+      </c>
+      <c r="F284" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G284" s="28"/>
+      <c r="H284" s="28"/>
+      <c r="I284" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J284" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="K284" s="28"/>
     </row>
     <row r="285" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="12" t="s">
-        <v>673</v>
-      </c>
-      <c r="B285" s="12" t="s">
-        <v>856</v>
-      </c>
-      <c r="C285" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="D285" s="20" t="s">
-        <v>740</v>
-      </c>
+        <v>869</v>
+      </c>
+      <c r="B285" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="C285" s="28"/>
+      <c r="D285" s="28"/>
       <c r="E285" s="12" t="s">
-        <v>803</v>
-      </c>
-      <c r="F285" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G285" s="12"/>
-      <c r="H285" s="12"/>
-      <c r="I285" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J285" s="12" t="s">
-        <v>543</v>
-      </c>
-      <c r="K285" s="12"/>
+        <v>871</v>
+      </c>
+      <c r="F285" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G285" s="28"/>
+      <c r="H285" s="28"/>
+      <c r="I285" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J285" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="K285" s="28"/>
     </row>
     <row r="286" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A286" s="12" t="s">
-        <v>742</v>
-      </c>
-      <c r="B286" s="12" t="s">
-        <v>856</v>
-      </c>
-      <c r="C286" s="20" t="s">
-        <v>743</v>
-      </c>
-      <c r="D286" s="12" t="s">
-        <v>740</v>
-      </c>
-      <c r="E286" s="12" t="s">
-        <v>744</v>
-      </c>
-      <c r="F286" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G286" s="13"/>
-      <c r="H286" s="13"/>
-      <c r="I286" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J286" s="13" t="s">
-        <v>543</v>
-      </c>
-      <c r="K286" s="12"/>
+      <c r="A286" s="24" t="s">
+        <v>575</v>
+      </c>
+      <c r="B286" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="C286" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="D286" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="E286" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="F286" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G286" s="24"/>
+      <c r="H286" s="24"/>
+      <c r="I286" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J286" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="K286" s="24"/>
     </row>
     <row r="287" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="12" t="s">
-        <v>742</v>
+        <v>716</v>
       </c>
       <c r="B287" s="12" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>743</v>
-      </c>
-      <c r="D287" s="12" t="s">
-        <v>740</v>
-      </c>
+        <v>717</v>
+      </c>
+      <c r="D287" s="12"/>
       <c r="E287" s="12" t="s">
-        <v>745</v>
-      </c>
-      <c r="F287" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G287" s="12"/>
-      <c r="H287" s="12"/>
-      <c r="I287" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J287" s="12" t="s">
-        <v>543</v>
+        <v>718</v>
+      </c>
+      <c r="F287" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G287" s="13"/>
+      <c r="H287" s="13"/>
+      <c r="I287" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J287" s="13" t="s">
+        <v>752</v>
       </c>
       <c r="K287" s="12"/>
     </row>
     <row r="288" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="12" t="s">
-        <v>757</v>
+        <v>673</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>848</v>
-      </c>
-      <c r="C288" s="12" t="s">
-        <v>758</v>
-      </c>
-      <c r="D288" s="12" t="s">
-        <v>723</v>
+        <v>856</v>
+      </c>
+      <c r="C288" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="D288" s="20" t="s">
+        <v>740</v>
       </c>
       <c r="E288" s="12" t="s">
-        <v>759</v>
+        <v>803</v>
       </c>
       <c r="F288" s="12" t="s">
         <v>497</v>
@@ -11618,40 +11631,127 @@
         <v>517</v>
       </c>
       <c r="J288" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K288" s="12"/>
+    </row>
+    <row r="289" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A289" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="B289" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C289" s="20" t="s">
+        <v>743</v>
+      </c>
+      <c r="D289" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="E289" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="F289" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G289" s="13"/>
+      <c r="H289" s="13"/>
+      <c r="I289" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J289" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="K289" s="12"/>
+    </row>
+    <row r="290" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A290" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="B290" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C290" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="D290" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="E290" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="F290" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G290" s="12"/>
+      <c r="H290" s="12"/>
+      <c r="I290" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J290" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K290" s="12"/>
+    </row>
+    <row r="291" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A291" s="12" t="s">
+        <v>757</v>
+      </c>
+      <c r="B291" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="C291" s="12" t="s">
+        <v>758</v>
+      </c>
+      <c r="D291" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="E291" s="12" t="s">
+        <v>759</v>
+      </c>
+      <c r="F291" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G291" s="12"/>
+      <c r="H291" s="12"/>
+      <c r="I291" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J291" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="K288" s="12"/>
-    </row>
-    <row r="289" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A289" s="28" t="s">
+      <c r="K291" s="12"/>
+    </row>
+    <row r="292" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A292" s="28" t="s">
         <v>901</v>
       </c>
-      <c r="B289" s="12" t="s">
+      <c r="B292" s="12" t="s">
         <v>902</v>
       </c>
-      <c r="C289" s="12" t="s">
+      <c r="C292" s="12" t="s">
         <v>903</v>
       </c>
-      <c r="D289" s="28"/>
-      <c r="E289" s="12" t="s">
+      <c r="D292" s="28"/>
+      <c r="E292" s="12" t="s">
         <v>904</v>
       </c>
-      <c r="F289" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G289" s="28"/>
-      <c r="H289" s="28"/>
-      <c r="I289" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J289" s="12" t="s">
+      <c r="F292" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G292" s="28"/>
+      <c r="H292" s="28"/>
+      <c r="I292" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J292" s="12" t="s">
         <v>905</v>
       </c>
-      <c r="K289" s="28"/>
+      <c r="K292" s="28"/>
     </row>
   </sheetData>
-  <sortState ref="A1:G408">
-    <sortCondition ref="A1:A408"/>
+  <sortState ref="A1:G411">
+    <sortCondition ref="A1:A411"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating Change Log and Daughter Board list for 2019_R2 release.
</commit_message>
<xml_diff>
--- a/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
+++ b/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSajikum\Documents\Linduino\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0C9D5-BB0B-4981-9CE1-0AFFD1B65E99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884AB2E7-4D6B-48AF-9203-405E2B3EEB83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="436900" windowHeight="101253" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="916">
   <si>
     <t>Description</t>
   </si>
@@ -2767,6 +2768,15 @@
   </si>
   <si>
     <t>Jothish Joseph Kalathil</t>
+  </si>
+  <si>
+    <t>LTC2971</t>
+  </si>
+  <si>
+    <t>DC2875A</t>
+  </si>
+  <si>
+    <t>Michael Peters</t>
   </si>
 </sst>
 </file>
@@ -3252,10 +3262,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A3:K292" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
-  <autoFilter ref="A3:K292" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState ref="A4:K291">
-    <sortCondition ref="A3:A291"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A3:K293" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
+  <autoFilter ref="A3:K293" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K292">
+    <sortCondition ref="A3:A292"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Product" dataDxfId="10" dataCellStyle="Normal"/>
@@ -3610,10 +3620,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L292"/>
+  <dimension ref="A1:L293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J271" sqref="J271"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -3624,8 +3634,8 @@
     <col min="4" max="4" width="6.1171875" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.234375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.17578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.87890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5859375" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.17578125" style="1"/>
   </cols>
@@ -3638,8 +3648,8 @@
         <v>518</v>
       </c>
       <c r="E1" s="14">
-        <f>(COUNTIF(I4:I292,"Done")/(COUNTA(A4:A292)-COUNTIF(H4:H292,"No")))</f>
-        <v>0.86497890295358648</v>
+        <f>(COUNTIF(I4:I293,"Done")/(COUNTA(A4:A293)-COUNTIF(H4:H293,"No")))</f>
+        <v>0.86554621848739499</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
@@ -3647,8 +3657,8 @@
         <v>519</v>
       </c>
       <c r="E2" s="14">
-        <f>(COUNTIF(F4:F292,"Yes")+(COUNTIF(F4:F292,"General"))+(COUNTIF(F4:F292,"Family")))/(COUNTA(A4:A292)-COUNTIF(H4:H292,"No"))</f>
-        <v>0.96624472573839659</v>
+        <f>(COUNTIF(F4:F293,"Yes")+(COUNTIF(F4:F293,"General"))+(COUNTIF(F4:F293,"Family")))/(COUNTA(A4:A293)-COUNTIF(H4:H293,"No"))</f>
+        <v>0.96638655462184875</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -9163,85 +9173,85 @@
       </c>
       <c r="K195" s="12"/>
     </row>
-    <row r="196" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="12" t="s">
-        <v>872</v>
+        <v>913</v>
       </c>
       <c r="B196" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C196" s="28"/>
-      <c r="D196" s="28"/>
+      <c r="C196" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D196" s="12" t="s">
+        <v>723</v>
+      </c>
       <c r="E196" s="12" t="s">
-        <v>873</v>
-      </c>
-      <c r="F196" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G196" s="29"/>
-      <c r="H196" s="28"/>
-      <c r="I196" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J196" s="12" t="s">
-        <v>874</v>
-      </c>
-      <c r="K196" s="28"/>
+        <v>914</v>
+      </c>
+      <c r="F196" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G196" s="13"/>
+      <c r="H196" s="13"/>
+      <c r="I196" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J196" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="K196" s="12"/>
     </row>
     <row r="197" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="12" t="s">
-        <v>736</v>
+        <v>872</v>
       </c>
       <c r="B197" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C197" s="20" t="s">
-        <v>737</v>
-      </c>
-      <c r="D197" s="12" t="s">
-        <v>740</v>
-      </c>
+      <c r="C197" s="28"/>
+      <c r="D197" s="28"/>
       <c r="E197" s="12" t="s">
-        <v>741</v>
-      </c>
-      <c r="F197" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G197" s="13"/>
-      <c r="H197" s="13"/>
-      <c r="I197" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J197" s="13" t="s">
-        <v>543</v>
-      </c>
-      <c r="K197" s="12"/>
+        <v>873</v>
+      </c>
+      <c r="F197" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G197" s="29"/>
+      <c r="H197" s="28"/>
+      <c r="I197" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J197" s="12" t="s">
+        <v>874</v>
+      </c>
+      <c r="K197" s="28"/>
     </row>
     <row r="198" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="12" t="s">
-        <v>631</v>
+        <v>736</v>
       </c>
       <c r="B198" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>656</v>
+        <v>737</v>
       </c>
       <c r="D198" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E198" s="12" t="s">
-        <v>666</v>
-      </c>
-      <c r="F198" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G198" s="12"/>
-      <c r="H198" s="12"/>
-      <c r="I198" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J198" s="12" t="s">
+        <v>741</v>
+      </c>
+      <c r="F198" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G198" s="13"/>
+      <c r="H198" s="13"/>
+      <c r="I198" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J198" s="13" t="s">
         <v>543</v>
       </c>
       <c r="K198" s="12"/>
@@ -9260,7 +9270,7 @@
         <v>740</v>
       </c>
       <c r="E199" s="12" t="s">
-        <v>632</v>
+        <v>666</v>
       </c>
       <c r="F199" s="12" t="s">
         <v>497</v>
@@ -9271,25 +9281,25 @@
         <v>517</v>
       </c>
       <c r="J199" s="12" t="s">
-        <v>735</v>
+        <v>543</v>
       </c>
       <c r="K199" s="12"/>
     </row>
     <row r="200" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="12" t="s">
-        <v>667</v>
+        <v>631</v>
       </c>
       <c r="B200" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C200" s="20" t="s">
-        <v>668</v>
+        <v>656</v>
       </c>
       <c r="D200" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E200" s="12" t="s">
-        <v>669</v>
+        <v>632</v>
       </c>
       <c r="F200" s="12" t="s">
         <v>497</v>
@@ -9300,33 +9310,31 @@
         <v>517</v>
       </c>
       <c r="J200" s="12" t="s">
-        <v>543</v>
+        <v>735</v>
       </c>
       <c r="K200" s="12"/>
     </row>
     <row r="201" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="12" t="s">
-        <v>738</v>
+        <v>667</v>
       </c>
       <c r="B201" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>739</v>
+        <v>668</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E201" s="12" t="s">
-        <v>746</v>
+        <v>669</v>
       </c>
       <c r="F201" s="12" t="s">
         <v>497</v>
       </c>
       <c r="G201" s="12"/>
-      <c r="H201" s="12" t="s">
-        <v>747</v>
-      </c>
+      <c r="H201" s="12"/>
       <c r="I201" s="12" t="s">
         <v>517</v>
       </c>
@@ -9337,25 +9345,27 @@
     </row>
     <row r="202" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="12" t="s">
-        <v>670</v>
+        <v>738</v>
       </c>
       <c r="B202" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C202" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="D202" s="20" t="s">
+        <v>739</v>
+      </c>
+      <c r="D202" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E202" s="12" t="s">
-        <v>672</v>
+        <v>746</v>
       </c>
       <c r="F202" s="12" t="s">
         <v>497</v>
       </c>
       <c r="G202" s="12"/>
-      <c r="H202" s="12"/>
+      <c r="H202" s="12" t="s">
+        <v>747</v>
+      </c>
       <c r="I202" s="12" t="s">
         <v>517</v>
       </c>
@@ -9366,19 +9376,19 @@
     </row>
     <row r="203" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="12" t="s">
-        <v>566</v>
+        <v>670</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>857</v>
-      </c>
-      <c r="C203" s="12" t="s">
-        <v>567</v>
-      </c>
-      <c r="D203" s="12" t="s">
-        <v>722</v>
+        <v>856</v>
+      </c>
+      <c r="C203" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="D203" s="20" t="s">
+        <v>740</v>
       </c>
       <c r="E203" s="12" t="s">
-        <v>568</v>
+        <v>672</v>
       </c>
       <c r="F203" s="12" t="s">
         <v>497</v>
@@ -9389,25 +9399,25 @@
         <v>517</v>
       </c>
       <c r="J203" s="12" t="s">
-        <v>640</v>
+        <v>543</v>
       </c>
       <c r="K203" s="12"/>
     </row>
     <row r="204" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="12" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="B204" s="12" t="s">
         <v>857</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>676</v>
+        <v>567</v>
       </c>
       <c r="D204" s="12" t="s">
         <v>722</v>
       </c>
       <c r="E204" s="12" t="s">
-        <v>802</v>
+        <v>568</v>
       </c>
       <c r="F204" s="12" t="s">
         <v>497</v>
@@ -9424,7 +9434,7 @@
     </row>
     <row r="205" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="12" t="s">
-        <v>748</v>
+        <v>580</v>
       </c>
       <c r="B205" s="12" t="s">
         <v>857</v>
@@ -9436,7 +9446,7 @@
         <v>722</v>
       </c>
       <c r="E205" s="12" t="s">
-        <v>749</v>
+        <v>802</v>
       </c>
       <c r="F205" s="12" t="s">
         <v>497</v>
@@ -9453,19 +9463,19 @@
     </row>
     <row r="206" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="12" t="s">
-        <v>28</v>
+        <v>748</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>27</v>
+        <v>676</v>
       </c>
       <c r="D206" s="12" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E206" s="12" t="s">
-        <v>26</v>
+        <v>749</v>
       </c>
       <c r="F206" s="12" t="s">
         <v>497</v>
@@ -9476,125 +9486,131 @@
         <v>517</v>
       </c>
       <c r="J206" s="12" t="s">
+        <v>640</v>
+      </c>
+      <c r="K206" s="12"/>
+    </row>
+    <row r="207" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B207" s="12" t="s">
+        <v>854</v>
+      </c>
+      <c r="C207" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D207" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="E207" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F207" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G207" s="12"/>
+      <c r="H207" s="12"/>
+      <c r="I207" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J207" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="K206" s="12"/>
-    </row>
-    <row r="207" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A207" s="13" t="s">
+      <c r="K207" s="12"/>
+    </row>
+    <row r="208" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B207" s="13" t="s">
+      <c r="B208" s="13" t="s">
         <v>854</v>
       </c>
-      <c r="C207" s="13" t="s">
+      <c r="C208" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="D207" s="13" t="s">
-        <v>723</v>
-      </c>
-      <c r="E207" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F207" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G207" s="13"/>
-      <c r="H207" s="13"/>
-      <c r="I207" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J207" s="13" t="s">
-        <v>551</v>
-      </c>
-      <c r="K207" s="13"/>
-    </row>
-    <row r="208" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A208" s="12" t="s">
-        <v>841</v>
-      </c>
-      <c r="B208" s="12" t="s">
-        <v>854</v>
-      </c>
-      <c r="C208" s="28" t="s">
-        <v>842</v>
       </c>
       <c r="D208" s="13" t="s">
         <v>723</v>
       </c>
-      <c r="E208" s="12" t="s">
+      <c r="E208" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F208" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G208" s="13"/>
+      <c r="H208" s="13"/>
+      <c r="I208" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J208" s="13" t="s">
+        <v>551</v>
+      </c>
+      <c r="K208" s="13"/>
+    </row>
+    <row r="209" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="B209" s="12" t="s">
+        <v>854</v>
+      </c>
+      <c r="C209" s="28" t="s">
+        <v>842</v>
+      </c>
+      <c r="D209" s="13" t="s">
+        <v>723</v>
+      </c>
+      <c r="E209" s="12" t="s">
         <v>843</v>
       </c>
-      <c r="F208" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G208" s="29"/>
-      <c r="H208" s="28"/>
-      <c r="I208" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J208" s="12" t="s">
+      <c r="F209" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G209" s="29"/>
+      <c r="H209" s="28"/>
+      <c r="I209" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J209" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="K208" s="28"/>
-    </row>
-    <row r="209" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A209" s="13" t="s">
+      <c r="K209" s="28"/>
+    </row>
+    <row r="210" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="B209" s="13"/>
-      <c r="C209" s="13" t="s">
+      <c r="B210" s="13"/>
+      <c r="C210" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="D209" s="13"/>
-      <c r="E209" s="13" t="s">
+      <c r="D210" s="13"/>
+      <c r="E210" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="F209" s="13" t="s">
+      <c r="F210" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="G209" s="13"/>
-      <c r="H209" s="13" t="s">
+      <c r="G210" s="13"/>
+      <c r="H210" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="I209" s="13"/>
-      <c r="J209" s="13"/>
-      <c r="K209" s="13"/>
-    </row>
-    <row r="210" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A210" s="12" t="s">
-        <v>400</v>
-      </c>
-      <c r="B210" s="12"/>
-      <c r="C210" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="D210" s="12"/>
-      <c r="E210" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="F210" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="G210" s="12"/>
-      <c r="H210" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="I210" s="12"/>
-      <c r="J210" s="12"/>
-      <c r="K210" s="12"/>
+      <c r="I210" s="13"/>
+      <c r="J210" s="13"/>
+      <c r="K210" s="13"/>
     </row>
     <row r="211" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="12" t="s">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="B211" s="12"/>
       <c r="C211" s="12" t="s">
-        <v>249</v>
+        <v>399</v>
       </c>
       <c r="D211" s="12"/>
       <c r="E211" s="12" t="s">
-        <v>248</v>
+        <v>398</v>
       </c>
       <c r="F211" s="12" t="s">
         <v>498</v>
@@ -9613,11 +9629,11 @@
       </c>
       <c r="B212" s="12"/>
       <c r="C212" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D212" s="12"/>
       <c r="E212" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F212" s="12" t="s">
         <v>498</v>
@@ -9632,15 +9648,15 @@
     </row>
     <row r="213" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="12" t="s">
-        <v>437</v>
+        <v>250</v>
       </c>
       <c r="B213" s="12"/>
       <c r="C213" s="12" t="s">
-        <v>436</v>
+        <v>252</v>
       </c>
       <c r="D213" s="12"/>
       <c r="E213" s="12" t="s">
-        <v>435</v>
+        <v>251</v>
       </c>
       <c r="F213" s="12" t="s">
         <v>498</v>
@@ -9655,15 +9671,15 @@
     </row>
     <row r="214" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="12" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="B214" s="12"/>
       <c r="C214" s="12" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="D214" s="12"/>
       <c r="E214" s="12" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="F214" s="12" t="s">
         <v>498</v>
@@ -9682,11 +9698,11 @@
       </c>
       <c r="B215" s="12"/>
       <c r="C215" s="12" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D215" s="12"/>
       <c r="E215" s="12" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F215" s="12" t="s">
         <v>498</v>
@@ -9701,15 +9717,15 @@
     </row>
     <row r="216" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="12" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B216" s="12"/>
       <c r="C216" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D216" s="12"/>
       <c r="E216" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F216" s="12" t="s">
         <v>498</v>
@@ -9724,15 +9740,15 @@
     </row>
     <row r="217" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="12" t="s">
-        <v>247</v>
+        <v>457</v>
       </c>
       <c r="B217" s="12"/>
       <c r="C217" s="12" t="s">
-        <v>246</v>
+        <v>456</v>
       </c>
       <c r="D217" s="12"/>
       <c r="E217" s="12" t="s">
-        <v>245</v>
+        <v>455</v>
       </c>
       <c r="F217" s="12" t="s">
         <v>498</v>
@@ -9747,15 +9763,15 @@
     </row>
     <row r="218" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="12" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B218" s="12"/>
       <c r="C218" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="D218" s="12"/>
       <c r="E218" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="F218" s="12" t="s">
         <v>498</v>
@@ -9774,11 +9790,11 @@
       </c>
       <c r="B219" s="12"/>
       <c r="C219" s="12" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D219" s="12"/>
       <c r="E219" s="12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F219" s="12" t="s">
         <v>498</v>
@@ -9792,73 +9808,73 @@
       <c r="K219" s="12"/>
     </row>
     <row r="220" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A220" s="13" t="s">
+      <c r="A220" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B220" s="12"/>
+      <c r="C220" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D220" s="12"/>
+      <c r="E220" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F220" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="G220" s="12"/>
+      <c r="H220" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I220" s="12"/>
+      <c r="J220" s="12"/>
+      <c r="K220" s="12"/>
+    </row>
+    <row r="221" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="B220" s="13"/>
-      <c r="C220" s="13" t="s">
+      <c r="B221" s="13"/>
+      <c r="C221" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="D220" s="13"/>
-      <c r="E220" s="13" t="s">
+      <c r="D221" s="13"/>
+      <c r="E221" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="F220" s="13" t="s">
+      <c r="F221" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="G220" s="13"/>
-      <c r="H220" s="13" t="s">
+      <c r="G221" s="13"/>
+      <c r="H221" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="I220" s="13"/>
-      <c r="J220" s="13"/>
-      <c r="K220" s="13"/>
-    </row>
-    <row r="221" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A221" s="12" t="s">
+      <c r="I221" s="13"/>
+      <c r="J221" s="13"/>
+      <c r="K221" s="13"/>
+    </row>
+    <row r="222" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B221" s="12"/>
-      <c r="C221" s="12" t="s">
+      <c r="B222" s="12"/>
+      <c r="C222" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="D221" s="12"/>
-      <c r="E221" s="12" t="s">
+      <c r="D222" s="12"/>
+      <c r="E222" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="F221" s="12" t="s">
+      <c r="F222" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="G221" s="12"/>
-      <c r="H221" s="12" t="s">
+      <c r="G222" s="12"/>
+      <c r="H222" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="I221" s="12"/>
-      <c r="J221" s="12"/>
-      <c r="K221" s="12"/>
-    </row>
-    <row r="222" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A222" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="B222" s="13"/>
-      <c r="C222" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="D222" s="13"/>
-      <c r="E222" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="F222" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="G222" s="13"/>
-      <c r="H222" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="I222" s="13"/>
-      <c r="J222" s="13"/>
-      <c r="K222" s="13"/>
+      <c r="I222" s="12"/>
+      <c r="J222" s="12"/>
+      <c r="K222" s="12"/>
     </row>
     <row r="223" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="13" t="s">
@@ -9866,11 +9882,11 @@
       </c>
       <c r="B223" s="13"/>
       <c r="C223" s="13" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D223" s="13"/>
       <c r="E223" s="13" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F223" s="13" t="s">
         <v>498</v>
@@ -9884,76 +9900,72 @@
       <c r="K223" s="13"/>
     </row>
     <row r="224" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A224" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="B224" s="12"/>
-      <c r="C224" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="D224" s="12"/>
-      <c r="E224" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="F224" s="12" t="s">
+      <c r="A224" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B224" s="13"/>
+      <c r="C224" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="D224" s="13"/>
+      <c r="E224" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="F224" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="G224" s="12"/>
-      <c r="H224" s="12" t="s">
+      <c r="G224" s="13"/>
+      <c r="H224" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="I224" s="12"/>
-      <c r="J224" s="12"/>
-      <c r="K224" s="12"/>
+      <c r="I224" s="13"/>
+      <c r="J224" s="13"/>
+      <c r="K224" s="13"/>
     </row>
     <row r="225" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="12" t="s">
-        <v>679</v>
-      </c>
-      <c r="B225" s="12" t="s">
-        <v>848</v>
-      </c>
-      <c r="C225" s="20" t="s">
-        <v>680</v>
-      </c>
-      <c r="D225" s="20" t="s">
-        <v>723</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="B225" s="12"/>
+      <c r="C225" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="D225" s="12"/>
       <c r="E225" s="12" t="s">
-        <v>681</v>
+        <v>307</v>
       </c>
       <c r="F225" s="12" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G225" s="12"/>
-      <c r="H225" s="12"/>
-      <c r="I225" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J225" s="12" t="s">
-        <v>682</v>
-      </c>
+      <c r="H225" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I225" s="12"/>
+      <c r="J225" s="12"/>
       <c r="K225" s="12"/>
     </row>
     <row r="226" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="12" t="s">
-        <v>683</v>
-      </c>
-      <c r="B226" s="12"/>
+        <v>679</v>
+      </c>
+      <c r="B226" s="12" t="s">
+        <v>848</v>
+      </c>
       <c r="C226" s="20" t="s">
-        <v>684</v>
-      </c>
-      <c r="D226" s="20"/>
+        <v>680</v>
+      </c>
+      <c r="D226" s="20" t="s">
+        <v>723</v>
+      </c>
       <c r="E226" s="12" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="F226" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G226" s="12"/>
-      <c r="H226" s="12" t="s">
-        <v>497</v>
-      </c>
+      <c r="H226" s="12"/>
       <c r="I226" s="12" t="s">
         <v>517</v>
       </c>
@@ -9964,56 +9976,52 @@
     </row>
     <row r="227" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="12" t="s">
-        <v>19</v>
+        <v>683</v>
       </c>
       <c r="B227" s="12"/>
-      <c r="C227" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D227" s="12"/>
+      <c r="C227" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="D227" s="20"/>
       <c r="E227" s="12" t="s">
-        <v>17</v>
+        <v>685</v>
       </c>
       <c r="F227" s="12" t="s">
         <v>498</v>
       </c>
       <c r="G227" s="12"/>
       <c r="H227" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="I227" s="12"/>
-      <c r="J227" s="12"/>
+        <v>497</v>
+      </c>
+      <c r="I227" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J227" s="12" t="s">
+        <v>682</v>
+      </c>
       <c r="K227" s="12"/>
     </row>
     <row r="228" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B228" s="12" t="s">
-        <v>848</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B228" s="12"/>
       <c r="C228" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D228" s="12" t="s">
-        <v>723</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D228" s="12"/>
       <c r="E228" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F228" s="13" t="s">
-        <v>499</v>
-      </c>
-      <c r="G228" s="13" t="s">
-        <v>858</v>
-      </c>
-      <c r="H228" s="13"/>
-      <c r="I228" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J228" s="13" t="s">
-        <v>527</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F228" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="G228" s="12"/>
+      <c r="H228" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I228" s="12"/>
+      <c r="J228" s="12"/>
       <c r="K228" s="12"/>
     </row>
     <row r="229" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -10024,92 +10032,96 @@
         <v>848</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="D229" s="12" t="s">
         <v>723</v>
       </c>
       <c r="E229" s="12" t="s">
-        <v>807</v>
-      </c>
-      <c r="F229" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G229" s="12"/>
-      <c r="H229" s="12"/>
-      <c r="I229" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J229" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F229" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="G229" s="13" t="s">
+        <v>858</v>
+      </c>
+      <c r="H229" s="13"/>
+      <c r="I229" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J229" s="13" t="s">
         <v>527</v>
       </c>
       <c r="K229" s="12"/>
     </row>
     <row r="230" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B230" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="B230" s="12" t="s">
+        <v>848</v>
+      </c>
       <c r="C230" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D230" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="D230" s="12" t="s">
+        <v>723</v>
+      </c>
       <c r="E230" s="12" t="s">
-        <v>172</v>
+        <v>807</v>
       </c>
       <c r="F230" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G230" s="12"/>
-      <c r="H230" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="I230" s="12"/>
-      <c r="J230" s="12"/>
+      <c r="H230" s="12"/>
+      <c r="I230" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J230" s="12" t="s">
+        <v>527</v>
+      </c>
       <c r="K230" s="12"/>
     </row>
     <row r="231" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="12" t="s">
-        <v>511</v>
-      </c>
-      <c r="B231" s="12" t="s">
-        <v>864</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B231" s="12"/>
       <c r="C231" s="12" t="s">
-        <v>808</v>
-      </c>
-      <c r="D231" s="12" t="s">
-        <v>723</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D231" s="12"/>
       <c r="E231" s="12" t="s">
-        <v>510</v>
+        <v>172</v>
       </c>
       <c r="F231" s="12" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G231" s="12"/>
-      <c r="H231" s="12"/>
-      <c r="I231" s="12" t="s">
-        <v>517</v>
-      </c>
+      <c r="H231" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I231" s="12"/>
       <c r="J231" s="12"/>
       <c r="K231" s="12"/>
     </row>
     <row r="232" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="12" t="s">
-        <v>534</v>
+        <v>511</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>540</v>
+        <v>808</v>
       </c>
       <c r="D232" s="12" t="s">
-        <v>740</v>
+        <v>723</v>
       </c>
       <c r="E232" s="12" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="F232" s="12" t="s">
         <v>497</v>
@@ -10119,26 +10131,24 @@
       <c r="I232" s="12" t="s">
         <v>517</v>
       </c>
-      <c r="J232" s="12" t="s">
-        <v>543</v>
-      </c>
+      <c r="J232" s="12"/>
       <c r="K232" s="12"/>
     </row>
     <row r="233" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B233" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D233" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E233" s="12" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F233" s="12" t="s">
         <v>497</v>
@@ -10154,291 +10164,297 @@
       <c r="K233" s="12"/>
     </row>
     <row r="234" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A234" s="13" t="s">
-        <v>536</v>
+      <c r="A234" s="12" t="s">
+        <v>535</v>
       </c>
       <c r="B234" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C234" s="13" t="s">
-        <v>542</v>
+      <c r="C234" s="12" t="s">
+        <v>541</v>
       </c>
       <c r="D234" s="12" t="s">
         <v>740</v>
       </c>
-      <c r="E234" s="13" t="s">
-        <v>537</v>
-      </c>
-      <c r="F234" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G234" s="13"/>
-      <c r="H234" s="13"/>
-      <c r="I234" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J234" s="13" t="s">
+      <c r="E234" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="F234" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G234" s="12"/>
+      <c r="H234" s="12"/>
+      <c r="I234" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J234" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="K234" s="13"/>
+      <c r="K234" s="12"/>
     </row>
     <row r="235" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A235" s="12" t="s">
-        <v>865</v>
+      <c r="A235" s="13" t="s">
+        <v>536</v>
       </c>
       <c r="B235" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C235" s="31" t="s">
-        <v>866</v>
+      <c r="C235" s="13" t="s">
+        <v>542</v>
       </c>
       <c r="D235" s="12" t="s">
         <v>740</v>
       </c>
-      <c r="E235" s="12" t="s">
-        <v>867</v>
-      </c>
-      <c r="F235" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G235" s="29"/>
-      <c r="H235" s="28"/>
+      <c r="E235" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="F235" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G235" s="13"/>
+      <c r="H235" s="13"/>
       <c r="I235" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="J235" s="28"/>
-      <c r="K235" s="28"/>
+      <c r="J235" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="K235" s="13"/>
     </row>
     <row r="236" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="12" t="s">
-        <v>693</v>
+        <v>865</v>
       </c>
       <c r="B236" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C236" s="12" t="s">
-        <v>694</v>
+      <c r="C236" s="31" t="s">
+        <v>866</v>
       </c>
       <c r="D236" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E236" s="12" t="s">
-        <v>674</v>
+        <v>867</v>
       </c>
       <c r="F236" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="G236" s="12"/>
-      <c r="H236" s="12"/>
-      <c r="I236" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J236" s="12" t="s">
-        <v>543</v>
-      </c>
-      <c r="K236" s="12"/>
+      <c r="G236" s="29"/>
+      <c r="H236" s="28"/>
+      <c r="I236" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J236" s="28"/>
+      <c r="K236" s="28"/>
     </row>
     <row r="237" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="B237" s="12"/>
+        <v>693</v>
+      </c>
+      <c r="B237" s="12" t="s">
+        <v>856</v>
+      </c>
       <c r="C237" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="D237" s="12"/>
+        <v>694</v>
+      </c>
+      <c r="D237" s="12" t="s">
+        <v>740</v>
+      </c>
       <c r="E237" s="12" t="s">
-        <v>344</v>
+        <v>674</v>
       </c>
       <c r="F237" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G237" s="12"/>
-      <c r="H237" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="I237" s="12"/>
-      <c r="J237" s="12"/>
-      <c r="K237" s="12" t="s">
-        <v>491</v>
-      </c>
+      <c r="H237" s="12"/>
+      <c r="I237" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J237" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K237" s="12"/>
     </row>
     <row r="238" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="12" t="s">
-        <v>406</v>
+        <v>346</v>
       </c>
       <c r="B238" s="12"/>
       <c r="C238" s="12" t="s">
-        <v>405</v>
+        <v>345</v>
       </c>
       <c r="D238" s="12"/>
       <c r="E238" s="12" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="F238" s="12" t="s">
         <v>498</v>
       </c>
       <c r="G238" s="12"/>
       <c r="H238" s="12" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="I238" s="12"/>
       <c r="J238" s="12"/>
-      <c r="K238" s="12"/>
+      <c r="K238" s="12" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="239" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="B239" s="12" t="s">
-        <v>854</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="B239" s="12"/>
       <c r="C239" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="D239" s="12" t="s">
-        <v>723</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="D239" s="12"/>
       <c r="E239" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="F239" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G239" s="13"/>
-      <c r="H239" s="13"/>
-      <c r="I239" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J239" s="30" t="s">
-        <v>809</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="F239" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="G239" s="12"/>
+      <c r="H239" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="I239" s="12"/>
+      <c r="J239" s="12"/>
       <c r="K239" s="12"/>
     </row>
     <row r="240" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="12" t="s">
-        <v>108</v>
+        <v>306</v>
       </c>
       <c r="B240" s="12" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>859</v>
+        <v>305</v>
       </c>
       <c r="D240" s="12" t="s">
         <v>723</v>
       </c>
       <c r="E240" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F240" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G240" s="12"/>
-      <c r="H240" s="12"/>
-      <c r="I240" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J240" s="12" t="s">
-        <v>686</v>
+        <v>304</v>
+      </c>
+      <c r="F240" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G240" s="13"/>
+      <c r="H240" s="13"/>
+      <c r="I240" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J240" s="30" t="s">
+        <v>809</v>
       </c>
       <c r="K240" s="12"/>
     </row>
     <row r="241" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B241" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="B241" s="12" t="s">
+        <v>848</v>
+      </c>
       <c r="C241" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D241" s="12"/>
+        <v>859</v>
+      </c>
+      <c r="D241" s="12" t="s">
+        <v>723</v>
+      </c>
       <c r="E241" s="12" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F241" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G241" s="12"/>
-      <c r="H241" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="I241" s="12"/>
-      <c r="J241" s="12"/>
+      <c r="H241" s="12"/>
+      <c r="I241" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J241" s="12" t="s">
+        <v>686</v>
+      </c>
       <c r="K241" s="12"/>
     </row>
     <row r="242" spans="1:11" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="B242" s="12" t="s">
-        <v>860</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B242" s="12"/>
       <c r="C242" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="D242" s="12" t="s">
-        <v>723</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D242" s="12"/>
       <c r="E242" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="F242" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G242" s="13"/>
-      <c r="H242" s="13"/>
-      <c r="I242" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J242" s="13" t="s">
-        <v>533</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F242" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="G242" s="12"/>
+      <c r="H242" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I242" s="12"/>
+      <c r="J242" s="12"/>
       <c r="K242" s="12"/>
     </row>
     <row r="243" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="B243" s="12"/>
+        <v>449</v>
+      </c>
+      <c r="B243" s="12" t="s">
+        <v>860</v>
+      </c>
       <c r="C243" s="12" t="s">
-        <v>311</v>
+        <v>448</v>
       </c>
       <c r="D243" s="12" t="s">
         <v>723</v>
       </c>
       <c r="E243" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="F243" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="G243" s="12"/>
-      <c r="H243" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="I243" s="12"/>
-      <c r="J243" s="12"/>
+        <v>447</v>
+      </c>
+      <c r="F243" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G243" s="13"/>
+      <c r="H243" s="13"/>
+      <c r="I243" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J243" s="13" t="s">
+        <v>533</v>
+      </c>
       <c r="K243" s="12"/>
     </row>
     <row r="244" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="12" t="s">
-        <v>282</v>
+        <v>312</v>
       </c>
       <c r="B244" s="12"/>
       <c r="C244" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="D244" s="12"/>
+        <v>311</v>
+      </c>
+      <c r="D244" s="12" t="s">
+        <v>723</v>
+      </c>
       <c r="E244" s="12" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="F244" s="12" t="s">
         <v>498</v>
       </c>
       <c r="G244" s="12"/>
       <c r="H244" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I244" s="12"/>
       <c r="J244" s="12"/>
@@ -10446,48 +10462,42 @@
     </row>
     <row r="245" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B245" s="12" t="s">
-        <v>860</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="B245" s="12"/>
       <c r="C245" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D245" s="12" t="s">
-        <v>723</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D245" s="12"/>
       <c r="E245" s="12" t="s">
-        <v>205</v>
+        <v>280</v>
       </c>
       <c r="F245" s="12" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G245" s="12"/>
-      <c r="H245" s="12"/>
-      <c r="I245" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J245" s="12" t="s">
-        <v>533</v>
-      </c>
+      <c r="H245" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I245" s="12"/>
+      <c r="J245" s="12"/>
       <c r="K245" s="12"/>
     </row>
     <row r="246" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="12" t="s">
-        <v>420</v>
+        <v>207</v>
       </c>
       <c r="B246" s="12" t="s">
         <v>860</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>419</v>
+        <v>206</v>
       </c>
       <c r="D246" s="12" t="s">
         <v>723</v>
       </c>
       <c r="E246" s="12" t="s">
-        <v>418</v>
+        <v>205</v>
       </c>
       <c r="F246" s="12" t="s">
         <v>497</v>
@@ -10504,19 +10514,19 @@
     </row>
     <row r="247" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="12" t="s">
-        <v>486</v>
+        <v>420</v>
       </c>
       <c r="B247" s="12" t="s">
         <v>860</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>485</v>
+        <v>419</v>
       </c>
       <c r="D247" s="12" t="s">
         <v>723</v>
       </c>
       <c r="E247" s="12" t="s">
-        <v>484</v>
+        <v>418</v>
       </c>
       <c r="F247" s="12" t="s">
         <v>497</v>
@@ -10532,84 +10542,84 @@
       <c r="K247" s="12"/>
     </row>
     <row r="248" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A248" s="13" t="s">
-        <v>144</v>
+      <c r="A248" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="B248" s="12" t="s">
         <v>860</v>
       </c>
-      <c r="C248" s="13" t="s">
+      <c r="C248" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="D248" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="E248" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="F248" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G248" s="12"/>
+      <c r="H248" s="12"/>
+      <c r="I248" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J248" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="K248" s="12"/>
+    </row>
+    <row r="249" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B249" s="12" t="s">
+        <v>860</v>
+      </c>
+      <c r="C249" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D248" s="13" t="s">
+      <c r="D249" s="13" t="s">
         <v>723</v>
       </c>
-      <c r="E248" s="13" t="s">
+      <c r="E249" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F248" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G248" s="13"/>
-      <c r="H248" s="13"/>
-      <c r="I248" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J248" s="13" t="s">
+      <c r="F249" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G249" s="13"/>
+      <c r="H249" s="13"/>
+      <c r="I249" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J249" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="K248" s="13"/>
-    </row>
-    <row r="249" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A249" s="12" t="s">
-        <v>558</v>
-      </c>
-      <c r="B249" s="12"/>
-      <c r="C249" s="12" t="s">
-        <v>695</v>
-      </c>
-      <c r="D249" s="12"/>
-      <c r="E249" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="F249" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="G249" s="12"/>
-      <c r="H249" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="I249" s="12" t="s">
-        <v>696</v>
-      </c>
-      <c r="J249" s="12" t="s">
-        <v>556</v>
-      </c>
-      <c r="K249" s="12"/>
+      <c r="K249" s="13"/>
     </row>
     <row r="250" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="12" t="s">
-        <v>560</v>
-      </c>
-      <c r="B250" s="12" t="s">
-        <v>860</v>
-      </c>
-      <c r="C250" s="20" t="s">
-        <v>645</v>
-      </c>
-      <c r="D250" s="20" t="s">
-        <v>723</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="B250" s="12"/>
+      <c r="C250" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="D250" s="12"/>
       <c r="E250" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F250" s="12" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G250" s="12"/>
-      <c r="H250" s="12"/>
+      <c r="H250" s="12" t="s">
+        <v>497</v>
+      </c>
       <c r="I250" s="12" t="s">
-        <v>517</v>
+        <v>696</v>
       </c>
       <c r="J250" s="12" t="s">
         <v>556</v>
@@ -10617,80 +10627,86 @@
       <c r="K250" s="12"/>
     </row>
     <row r="251" spans="1:11" s="15" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A251" s="13" t="s">
+      <c r="A251" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="B251" s="12" t="s">
+        <v>860</v>
+      </c>
+      <c r="C251" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="D251" s="20" t="s">
+        <v>723</v>
+      </c>
+      <c r="E251" s="12" t="s">
+        <v>561</v>
+      </c>
+      <c r="F251" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G251" s="12"/>
+      <c r="H251" s="12"/>
+      <c r="I251" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J251" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="K251" s="12"/>
+    </row>
+    <row r="252" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="13" t="s">
         <v>592</v>
       </c>
-      <c r="B251" s="13"/>
-      <c r="C251" s="13" t="s">
+      <c r="B252" s="13"/>
+      <c r="C252" s="13" t="s">
         <v>660</v>
       </c>
-      <c r="D251" s="13"/>
-      <c r="E251" s="13" t="s">
+      <c r="D252" s="13"/>
+      <c r="E252" s="13" t="s">
         <v>661</v>
       </c>
-      <c r="F251" s="13" t="s">
+      <c r="F252" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="G251" s="13"/>
-      <c r="H251" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="I251" s="13" t="s">
+      <c r="G252" s="13"/>
+      <c r="H252" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="I252" s="13" t="s">
         <v>659</v>
       </c>
-      <c r="J251" s="13" t="s">
+      <c r="J252" s="13" t="s">
         <v>556</v>
       </c>
-      <c r="K251" s="13"/>
-    </row>
-    <row r="252" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A252" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="B252" s="12"/>
-      <c r="C252" s="12" t="s">
-        <v>657</v>
-      </c>
-      <c r="D252" s="12"/>
-      <c r="E252" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="F252" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="G252" s="12"/>
-      <c r="H252" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="I252" s="12" t="s">
-        <v>659</v>
-      </c>
-      <c r="J252" s="12" t="s">
-        <v>556</v>
-      </c>
-      <c r="K252" s="12"/>
+      <c r="K252" s="13"/>
     </row>
     <row r="253" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="12" t="s">
-        <v>409</v>
+        <v>591</v>
       </c>
       <c r="B253" s="12"/>
       <c r="C253" s="12" t="s">
-        <v>408</v>
+        <v>657</v>
       </c>
       <c r="D253" s="12"/>
       <c r="E253" s="12" t="s">
-        <v>407</v>
+        <v>658</v>
       </c>
       <c r="F253" s="12" t="s">
         <v>498</v>
       </c>
       <c r="G253" s="12"/>
       <c r="H253" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="I253" s="12"/>
-      <c r="J253" s="12"/>
+        <v>497</v>
+      </c>
+      <c r="I253" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="J253" s="12" t="s">
+        <v>556</v>
+      </c>
       <c r="K253" s="12"/>
     </row>
     <row r="254" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -10699,11 +10715,11 @@
       </c>
       <c r="B254" s="12"/>
       <c r="C254" s="12" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D254" s="12"/>
       <c r="E254" s="12" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F254" s="12" t="s">
         <v>498</v>
@@ -10718,258 +10734,258 @@
     </row>
     <row r="255" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="12" t="s">
-        <v>562</v>
-      </c>
-      <c r="B255" s="12" t="s">
-        <v>863</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="B255" s="12"/>
       <c r="C255" s="12" t="s">
-        <v>655</v>
+        <v>411</v>
       </c>
       <c r="D255" s="12"/>
       <c r="E255" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="F255" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="G255" s="12"/>
+      <c r="H255" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I255" s="12"/>
+      <c r="J255" s="12"/>
+      <c r="K255" s="12"/>
+    </row>
+    <row r="256" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A256" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="B256" s="12" t="s">
+        <v>863</v>
+      </c>
+      <c r="C256" s="12" t="s">
+        <v>655</v>
+      </c>
+      <c r="D256" s="12"/>
+      <c r="E256" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="F255" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G255" s="12"/>
-      <c r="H255" s="12"/>
-      <c r="I255" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J255" s="12" t="s">
+      <c r="F256" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G256" s="12"/>
+      <c r="H256" s="12"/>
+      <c r="I256" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J256" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="K255" s="12"/>
-    </row>
-    <row r="256" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A256" s="24" t="s">
+      <c r="K256" s="12"/>
+    </row>
+    <row r="257" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A257" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="B256" s="12" t="s">
+      <c r="B257" s="12" t="s">
         <v>864</v>
       </c>
-      <c r="C256" s="24" t="s">
+      <c r="C257" s="24" t="s">
         <v>690</v>
       </c>
-      <c r="D256" s="24"/>
-      <c r="E256" s="24" t="s">
+      <c r="D257" s="24"/>
+      <c r="E257" s="24" t="s">
         <v>689</v>
       </c>
-      <c r="F256" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="G256" s="24"/>
-      <c r="H256" s="24"/>
-      <c r="I256" s="24" t="s">
+      <c r="F257" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G257" s="24"/>
+      <c r="H257" s="24"/>
+      <c r="I257" s="24" t="s">
         <v>810</v>
       </c>
-      <c r="J256" s="24" t="s">
+      <c r="J257" s="24" t="s">
         <v>732</v>
       </c>
-      <c r="K256" s="24"/>
-    </row>
-    <row r="257" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A257" s="12" t="s">
+      <c r="K257" s="24"/>
+    </row>
+    <row r="258" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A258" s="12" t="s">
         <v>898</v>
       </c>
-      <c r="B257" s="12" t="s">
+      <c r="B258" s="12" t="s">
         <v>861</v>
       </c>
-      <c r="C257" s="15" t="s">
+      <c r="C258" s="15" t="s">
         <v>899</v>
       </c>
-      <c r="D257" s="28"/>
-      <c r="E257" s="12" t="s">
+      <c r="D258" s="28"/>
+      <c r="E258" s="12" t="s">
         <v>900</v>
       </c>
-      <c r="F257" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G257" s="28"/>
-      <c r="H257" s="28"/>
-      <c r="I257" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J257" s="12" t="s">
+      <c r="F258" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G258" s="28"/>
+      <c r="H258" s="28"/>
+      <c r="I258" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J258" s="12" t="s">
         <v>732</v>
       </c>
-      <c r="K257" s="28"/>
-    </row>
-    <row r="258" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A258" s="24" t="s">
-        <v>688</v>
-      </c>
-      <c r="B258" s="24" t="s">
-        <v>861</v>
-      </c>
-      <c r="C258" s="24" t="s">
-        <v>691</v>
-      </c>
-      <c r="D258" s="24" t="s">
-        <v>722</v>
-      </c>
-      <c r="E258" s="24" t="s">
-        <v>692</v>
-      </c>
-      <c r="F258" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G258" s="25"/>
-      <c r="H258" s="25"/>
-      <c r="I258" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J258" s="25" t="s">
-        <v>732</v>
-      </c>
-      <c r="K258" s="24"/>
+      <c r="K258" s="28"/>
     </row>
     <row r="259" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="24" t="s">
-        <v>544</v>
+        <v>688</v>
       </c>
       <c r="B259" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C259" s="24" t="s">
-        <v>546</v>
+        <v>691</v>
       </c>
       <c r="D259" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E259" s="24" t="s">
-        <v>545</v>
-      </c>
-      <c r="F259" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="G259" s="24"/>
-      <c r="H259" s="24"/>
-      <c r="I259" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J259" s="24" t="s">
-        <v>523</v>
+        <v>692</v>
+      </c>
+      <c r="F259" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="G259" s="25"/>
+      <c r="H259" s="25"/>
+      <c r="I259" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J259" s="25" t="s">
+        <v>732</v>
       </c>
       <c r="K259" s="24"/>
     </row>
     <row r="260" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="24" t="s">
-        <v>598</v>
-      </c>
-      <c r="B260" s="24"/>
+        <v>544</v>
+      </c>
+      <c r="B260" s="24" t="s">
+        <v>861</v>
+      </c>
       <c r="C260" s="24" t="s">
-        <v>599</v>
-      </c>
-      <c r="D260" s="24"/>
+        <v>546</v>
+      </c>
+      <c r="D260" s="24" t="s">
+        <v>722</v>
+      </c>
       <c r="E260" s="24" t="s">
-        <v>202</v>
+        <v>545</v>
       </c>
       <c r="F260" s="24" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G260" s="24"/>
-      <c r="H260" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="I260" s="24"/>
+      <c r="H260" s="24"/>
+      <c r="I260" s="24" t="s">
+        <v>517</v>
+      </c>
       <c r="J260" s="24" t="s">
-        <v>596</v>
+        <v>523</v>
       </c>
       <c r="K260" s="24"/>
     </row>
     <row r="261" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="24" t="s">
-        <v>526</v>
-      </c>
-      <c r="B261" s="24" t="s">
-        <v>861</v>
-      </c>
+        <v>598</v>
+      </c>
+      <c r="B261" s="24"/>
       <c r="C261" s="24" t="s">
-        <v>646</v>
-      </c>
-      <c r="D261" s="24" t="s">
-        <v>722</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="D261" s="24"/>
       <c r="E261" s="24" t="s">
-        <v>648</v>
-      </c>
-      <c r="F261" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G261" s="25"/>
-      <c r="H261" s="25"/>
-      <c r="I261" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J261" s="25" t="s">
-        <v>641</v>
+        <v>202</v>
+      </c>
+      <c r="F261" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="G261" s="24"/>
+      <c r="H261" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="I261" s="24"/>
+      <c r="J261" s="24" t="s">
+        <v>596</v>
       </c>
       <c r="K261" s="24"/>
     </row>
     <row r="262" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="24" t="s">
-        <v>642</v>
-      </c>
-      <c r="B262" s="24"/>
+        <v>526</v>
+      </c>
+      <c r="B262" s="24" t="s">
+        <v>861</v>
+      </c>
       <c r="C262" s="24" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D262" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E262" s="24" t="s">
-        <v>649</v>
-      </c>
-      <c r="F262" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="G262" s="24"/>
-      <c r="H262" s="24"/>
-      <c r="I262" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J262" s="24" t="s">
+        <v>648</v>
+      </c>
+      <c r="F262" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="G262" s="25"/>
+      <c r="H262" s="25"/>
+      <c r="I262" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J262" s="25" t="s">
         <v>641</v>
       </c>
       <c r="K262" s="24"/>
     </row>
     <row r="263" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="24" t="s">
-        <v>211</v>
+        <v>642</v>
       </c>
       <c r="B263" s="24"/>
       <c r="C263" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="D263" s="24"/>
+        <v>647</v>
+      </c>
+      <c r="D263" s="24" t="s">
+        <v>722</v>
+      </c>
       <c r="E263" s="24" t="s">
-        <v>209</v>
+        <v>649</v>
       </c>
       <c r="F263" s="24" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G263" s="24"/>
-      <c r="H263" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I263" s="24"/>
-      <c r="J263" s="24"/>
+      <c r="H263" s="24"/>
+      <c r="I263" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J263" s="24" t="s">
+        <v>641</v>
+      </c>
       <c r="K263" s="24"/>
     </row>
     <row r="264" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="24" t="s">
-        <v>343</v>
+        <v>211</v>
       </c>
       <c r="B264" s="24"/>
       <c r="C264" s="24" t="s">
-        <v>342</v>
+        <v>210</v>
       </c>
       <c r="D264" s="24"/>
       <c r="E264" s="24" t="s">
-        <v>341</v>
+        <v>209</v>
       </c>
       <c r="F264" s="24" t="s">
         <v>498</v>
@@ -10984,44 +11000,40 @@
     </row>
     <row r="265" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="24" t="s">
-        <v>621</v>
-      </c>
-      <c r="B265" s="24" t="s">
-        <v>862</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="B265" s="24"/>
       <c r="C265" s="24" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="D265" s="24"/>
       <c r="E265" s="24" t="s">
-        <v>190</v>
+        <v>341</v>
       </c>
       <c r="F265" s="24" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G265" s="24"/>
-      <c r="H265" s="24"/>
-      <c r="I265" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J265" s="24" t="s">
-        <v>620</v>
-      </c>
+      <c r="H265" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="I265" s="24"/>
+      <c r="J265" s="24"/>
       <c r="K265" s="24"/>
     </row>
     <row r="266" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="24" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B266" s="24" t="s">
         <v>862</v>
       </c>
       <c r="C266" s="24" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D266" s="24"/>
       <c r="E266" s="24" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="F266" s="24" t="s">
         <v>497</v>
@@ -11038,38 +11050,42 @@
     </row>
     <row r="267" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="24" t="s">
-        <v>623</v>
-      </c>
-      <c r="B267" s="24"/>
+        <v>622</v>
+      </c>
+      <c r="B267" s="24" t="s">
+        <v>862</v>
+      </c>
       <c r="C267" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D267" s="24"/>
       <c r="E267" s="24" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F267" s="24" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G267" s="24"/>
-      <c r="H267" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I267" s="24"/>
-      <c r="J267" s="24"/>
+      <c r="H267" s="24"/>
+      <c r="I267" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J267" s="24" t="s">
+        <v>620</v>
+      </c>
       <c r="K267" s="24"/>
     </row>
     <row r="268" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="24" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B268" s="24"/>
       <c r="C268" s="24" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="D268" s="24"/>
       <c r="E268" s="24" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="F268" s="24" t="s">
         <v>498</v>
@@ -11084,44 +11100,40 @@
     </row>
     <row r="269" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="24" t="s">
-        <v>503</v>
-      </c>
-      <c r="B269" s="24" t="s">
-        <v>862</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="B269" s="24"/>
       <c r="C269" s="24" t="s">
-        <v>502</v>
+        <v>100</v>
       </c>
       <c r="D269" s="24"/>
       <c r="E269" s="24" t="s">
-        <v>501</v>
+        <v>99</v>
       </c>
       <c r="F269" s="24" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G269" s="24"/>
-      <c r="H269" s="24"/>
-      <c r="I269" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J269" s="24" t="s">
-        <v>620</v>
-      </c>
+      <c r="H269" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="I269" s="24"/>
+      <c r="J269" s="24"/>
       <c r="K269" s="24"/>
     </row>
     <row r="270" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="24" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B270" s="24" t="s">
         <v>862</v>
       </c>
       <c r="C270" s="24" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D270" s="24"/>
       <c r="E270" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F270" s="24" t="s">
         <v>497</v>
@@ -11137,35 +11149,35 @@
       <c r="K270" s="24"/>
     </row>
     <row r="271" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A271" s="12" t="s">
-        <v>906</v>
+      <c r="A271" s="24" t="s">
+        <v>506</v>
       </c>
       <c r="B271" s="24" t="s">
         <v>862</v>
       </c>
       <c r="C271" s="24" t="s">
-        <v>805</v>
-      </c>
-      <c r="D271" s="28"/>
-      <c r="E271" s="12" t="s">
-        <v>909</v>
+        <v>505</v>
+      </c>
+      <c r="D271" s="24"/>
+      <c r="E271" s="24" t="s">
+        <v>504</v>
       </c>
       <c r="F271" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G271" s="28"/>
-      <c r="H271" s="28"/>
+      <c r="G271" s="24"/>
+      <c r="H271" s="24"/>
       <c r="I271" s="24" t="s">
         <v>517</v>
       </c>
-      <c r="J271" s="12" t="s">
-        <v>912</v>
-      </c>
-      <c r="K271" s="28"/>
+      <c r="J271" s="24" t="s">
+        <v>620</v>
+      </c>
+      <c r="K271" s="24"/>
     </row>
     <row r="272" spans="1:12" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A272" s="24" t="s">
-        <v>804</v>
+      <c r="A272" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="B272" s="24" t="s">
         <v>862</v>
@@ -11173,27 +11185,27 @@
       <c r="C272" s="24" t="s">
         <v>805</v>
       </c>
-      <c r="D272" s="24"/>
-      <c r="E272" s="24" t="s">
-        <v>806</v>
+      <c r="D272" s="28"/>
+      <c r="E272" s="12" t="s">
+        <v>909</v>
       </c>
       <c r="F272" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G272" s="24"/>
-      <c r="H272" s="24"/>
+      <c r="G272" s="28"/>
+      <c r="H272" s="28"/>
       <c r="I272" s="24" t="s">
         <v>517</v>
       </c>
-      <c r="J272" s="24" t="s">
-        <v>620</v>
-      </c>
-      <c r="K272" s="24"/>
+      <c r="J272" s="12" t="s">
+        <v>912</v>
+      </c>
+      <c r="K272" s="28"/>
       <c r="L272" s="19"/>
     </row>
     <row r="273" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A273" s="12" t="s">
-        <v>907</v>
+      <c r="A273" s="24" t="s">
+        <v>804</v>
       </c>
       <c r="B273" s="24" t="s">
         <v>862</v>
@@ -11201,34 +11213,36 @@
       <c r="C273" s="24" t="s">
         <v>805</v>
       </c>
-      <c r="D273" s="28"/>
-      <c r="E273" s="12" t="s">
-        <v>910</v>
+      <c r="D273" s="24"/>
+      <c r="E273" s="24" t="s">
+        <v>806</v>
       </c>
       <c r="F273" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G273" s="28"/>
-      <c r="H273" s="28"/>
+      <c r="G273" s="24"/>
+      <c r="H273" s="24"/>
       <c r="I273" s="24" t="s">
         <v>517</v>
       </c>
-      <c r="J273" s="12" t="s">
-        <v>912</v>
-      </c>
-      <c r="K273" s="28"/>
+      <c r="J273" s="24" t="s">
+        <v>620</v>
+      </c>
+      <c r="K273" s="24"/>
     </row>
     <row r="274" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="12" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B274" s="24" t="s">
         <v>862</v>
       </c>
-      <c r="C274" s="28"/>
+      <c r="C274" s="24" t="s">
+        <v>805</v>
+      </c>
       <c r="D274" s="28"/>
       <c r="E274" s="12" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="F274" s="24" t="s">
         <v>497</v>
@@ -11244,72 +11258,68 @@
       <c r="K274" s="28"/>
     </row>
     <row r="275" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A275" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D275" s="24"/>
-      <c r="E275" s="24" t="s">
-        <v>23</v>
+      <c r="A275" s="12" t="s">
+        <v>908</v>
+      </c>
+      <c r="B275" s="24" t="s">
+        <v>862</v>
+      </c>
+      <c r="C275" s="28"/>
+      <c r="D275" s="28"/>
+      <c r="E275" s="12" t="s">
+        <v>911</v>
       </c>
       <c r="F275" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="G275" s="24"/>
-      <c r="H275" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I275" s="24"/>
-      <c r="J275" s="24"/>
-      <c r="K275" s="24"/>
+        <v>497</v>
+      </c>
+      <c r="G275" s="28"/>
+      <c r="H275" s="28"/>
+      <c r="I275" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J275" s="12" t="s">
+        <v>912</v>
+      </c>
+      <c r="K275" s="28"/>
     </row>
     <row r="276" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="B276" s="24" t="s">
-        <v>861</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B276" s="24"/>
       <c r="C276" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="D276" s="24" t="s">
-        <v>722</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D276" s="24"/>
       <c r="E276" s="24" t="s">
-        <v>811</v>
-      </c>
-      <c r="F276" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="G276" s="25"/>
-      <c r="H276" s="25"/>
-      <c r="I276" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="J276" s="25" t="s">
-        <v>551</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F276" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="G276" s="24"/>
+      <c r="H276" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="I276" s="24"/>
+      <c r="J276" s="24"/>
       <c r="K276" s="24"/>
     </row>
     <row r="277" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="24" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B277" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C277" s="24" t="s">
-        <v>812</v>
+        <v>508</v>
       </c>
       <c r="D277" s="24" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E277" s="24" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F277" s="25" t="s">
         <v>497</v>
@@ -11326,48 +11336,48 @@
     </row>
     <row r="278" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="24" t="s">
-        <v>106</v>
+        <v>507</v>
       </c>
       <c r="B278" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C278" s="24" t="s">
-        <v>105</v>
+        <v>812</v>
       </c>
       <c r="D278" s="24" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="E278" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="F278" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="G278" s="24"/>
-      <c r="H278" s="24"/>
-      <c r="I278" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="J278" s="24" t="s">
-        <v>549</v>
+        <v>813</v>
+      </c>
+      <c r="F278" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="G278" s="25"/>
+      <c r="H278" s="25"/>
+      <c r="I278" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="J278" s="25" t="s">
+        <v>551</v>
       </c>
       <c r="K278" s="24"/>
     </row>
     <row r="279" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="24" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="B279" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C279" s="24" t="s">
-        <v>617</v>
+        <v>105</v>
       </c>
       <c r="D279" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E279" s="24" t="s">
-        <v>618</v>
+        <v>104</v>
       </c>
       <c r="F279" s="24" t="s">
         <v>497</v>
@@ -11380,25 +11390,23 @@
       <c r="J279" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K279" s="24" t="s">
-        <v>490</v>
-      </c>
+      <c r="K279" s="24"/>
     </row>
     <row r="280" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="24" t="s">
-        <v>570</v>
+        <v>38</v>
       </c>
       <c r="B280" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C280" s="24" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D280" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E280" s="24" t="s">
-        <v>571</v>
+        <v>618</v>
       </c>
       <c r="F280" s="24" t="s">
         <v>497</v>
@@ -11411,23 +11419,25 @@
       <c r="J280" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K280" s="24"/>
+      <c r="K280" s="24" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="281" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="24" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B281" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C281" s="24" t="s">
-        <v>697</v>
+        <v>615</v>
       </c>
       <c r="D281" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E281" s="24" t="s">
-        <v>698</v>
+        <v>571</v>
       </c>
       <c r="F281" s="24" t="s">
         <v>497</v>
@@ -11444,19 +11454,19 @@
     </row>
     <row r="282" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="24" t="s">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="B282" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C282" s="24" t="s">
-        <v>616</v>
+        <v>697</v>
       </c>
       <c r="D282" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E282" s="24" t="s">
-        <v>548</v>
+        <v>698</v>
       </c>
       <c r="F282" s="24" t="s">
         <v>497</v>
@@ -11473,19 +11483,19 @@
     </row>
     <row r="283" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="24" t="s">
-        <v>578</v>
+        <v>547</v>
       </c>
       <c r="B283" s="24" t="s">
         <v>861</v>
       </c>
       <c r="C283" s="24" t="s">
-        <v>662</v>
+        <v>616</v>
       </c>
       <c r="D283" s="24" t="s">
         <v>722</v>
       </c>
       <c r="E283" s="24" t="s">
-        <v>725</v>
+        <v>548</v>
       </c>
       <c r="F283" s="24" t="s">
         <v>497</v>
@@ -11501,33 +11511,37 @@
       <c r="K283" s="24"/>
     </row>
     <row r="284" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A284" s="12" t="s">
-        <v>868</v>
+      <c r="A284" s="24" t="s">
+        <v>578</v>
       </c>
       <c r="B284" s="24" t="s">
         <v>861</v>
       </c>
-      <c r="C284" s="28"/>
-      <c r="D284" s="28"/>
-      <c r="E284" s="12" t="s">
-        <v>870</v>
+      <c r="C284" s="24" t="s">
+        <v>662</v>
+      </c>
+      <c r="D284" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="E284" s="24" t="s">
+        <v>725</v>
       </c>
       <c r="F284" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G284" s="28"/>
-      <c r="H284" s="28"/>
+      <c r="G284" s="24"/>
+      <c r="H284" s="24"/>
       <c r="I284" s="24" t="s">
         <v>517</v>
       </c>
       <c r="J284" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K284" s="28"/>
+      <c r="K284" s="24"/>
     </row>
     <row r="285" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="12" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B285" s="24" t="s">
         <v>861</v>
@@ -11535,7 +11549,7 @@
       <c r="C285" s="28"/>
       <c r="D285" s="28"/>
       <c r="E285" s="12" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F285" s="24" t="s">
         <v>497</v>
@@ -11551,115 +11565,111 @@
       <c r="K285" s="28"/>
     </row>
     <row r="286" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A286" s="24" t="s">
-        <v>575</v>
+      <c r="A286" s="12" t="s">
+        <v>869</v>
       </c>
       <c r="B286" s="24" t="s">
         <v>861</v>
       </c>
-      <c r="C286" s="24" t="s">
-        <v>619</v>
-      </c>
-      <c r="D286" s="24" t="s">
-        <v>722</v>
-      </c>
-      <c r="E286" s="24" t="s">
-        <v>576</v>
+      <c r="C286" s="28"/>
+      <c r="D286" s="28"/>
+      <c r="E286" s="12" t="s">
+        <v>871</v>
       </c>
       <c r="F286" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="G286" s="24"/>
-      <c r="H286" s="24"/>
+      <c r="G286" s="28"/>
+      <c r="H286" s="28"/>
       <c r="I286" s="24" t="s">
         <v>517</v>
       </c>
       <c r="J286" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="K286" s="24"/>
+      <c r="K286" s="28"/>
     </row>
     <row r="287" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A287" s="12" t="s">
-        <v>716</v>
-      </c>
-      <c r="B287" s="12" t="s">
-        <v>847</v>
-      </c>
-      <c r="C287" s="12" t="s">
-        <v>717</v>
-      </c>
-      <c r="D287" s="12"/>
-      <c r="E287" s="12" t="s">
-        <v>718</v>
-      </c>
-      <c r="F287" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G287" s="13"/>
-      <c r="H287" s="13"/>
-      <c r="I287" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J287" s="13" t="s">
-        <v>752</v>
-      </c>
-      <c r="K287" s="12"/>
+      <c r="A287" s="24" t="s">
+        <v>575</v>
+      </c>
+      <c r="B287" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="C287" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="D287" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="E287" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="F287" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="G287" s="24"/>
+      <c r="H287" s="24"/>
+      <c r="I287" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="J287" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="K287" s="24"/>
     </row>
     <row r="288" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="12" t="s">
-        <v>673</v>
+        <v>716</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>856</v>
-      </c>
-      <c r="C288" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="D288" s="20" t="s">
-        <v>740</v>
-      </c>
+        <v>847</v>
+      </c>
+      <c r="C288" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="D288" s="12"/>
       <c r="E288" s="12" t="s">
-        <v>803</v>
-      </c>
-      <c r="F288" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G288" s="12"/>
-      <c r="H288" s="12"/>
-      <c r="I288" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J288" s="12" t="s">
-        <v>543</v>
+        <v>718</v>
+      </c>
+      <c r="F288" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G288" s="13"/>
+      <c r="H288" s="13"/>
+      <c r="I288" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J288" s="13" t="s">
+        <v>752</v>
       </c>
       <c r="K288" s="12"/>
     </row>
     <row r="289" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="12" t="s">
-        <v>742</v>
+        <v>673</v>
       </c>
       <c r="B289" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C289" s="20" t="s">
-        <v>743</v>
-      </c>
-      <c r="D289" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="D289" s="20" t="s">
         <v>740</v>
       </c>
       <c r="E289" s="12" t="s">
-        <v>744</v>
-      </c>
-      <c r="F289" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G289" s="13"/>
-      <c r="H289" s="13"/>
-      <c r="I289" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J289" s="13" t="s">
+        <v>803</v>
+      </c>
+      <c r="F289" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G289" s="12"/>
+      <c r="H289" s="12"/>
+      <c r="I289" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J289" s="12" t="s">
         <v>543</v>
       </c>
       <c r="K289" s="12"/>
@@ -11671,43 +11681,43 @@
       <c r="B290" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C290" s="12" t="s">
+      <c r="C290" s="20" t="s">
         <v>743</v>
       </c>
       <c r="D290" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E290" s="12" t="s">
-        <v>745</v>
-      </c>
-      <c r="F290" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G290" s="12"/>
-      <c r="H290" s="12"/>
-      <c r="I290" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J290" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="F290" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G290" s="13"/>
+      <c r="H290" s="13"/>
+      <c r="I290" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J290" s="13" t="s">
         <v>543</v>
       </c>
       <c r="K290" s="12"/>
     </row>
     <row r="291" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="12" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="B291" s="12" t="s">
-        <v>848</v>
+        <v>856</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>758</v>
+        <v>743</v>
       </c>
       <c r="D291" s="12" t="s">
-        <v>723</v>
+        <v>740</v>
       </c>
       <c r="E291" s="12" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="F291" s="12" t="s">
         <v>497</v>
@@ -11718,40 +11728,69 @@
         <v>517</v>
       </c>
       <c r="J291" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K291" s="12"/>
+    </row>
+    <row r="292" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A292" s="12" t="s">
+        <v>757</v>
+      </c>
+      <c r="B292" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="C292" s="12" t="s">
+        <v>758</v>
+      </c>
+      <c r="D292" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="E292" s="12" t="s">
+        <v>759</v>
+      </c>
+      <c r="F292" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G292" s="12"/>
+      <c r="H292" s="12"/>
+      <c r="I292" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J292" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="K291" s="12"/>
-    </row>
-    <row r="292" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A292" s="28" t="s">
+      <c r="K292" s="12"/>
+    </row>
+    <row r="293" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A293" s="28" t="s">
         <v>901</v>
       </c>
-      <c r="B292" s="12" t="s">
+      <c r="B293" s="12" t="s">
         <v>902</v>
       </c>
-      <c r="C292" s="12" t="s">
+      <c r="C293" s="12" t="s">
         <v>903</v>
       </c>
-      <c r="D292" s="28"/>
-      <c r="E292" s="12" t="s">
+      <c r="D293" s="28"/>
+      <c r="E293" s="12" t="s">
         <v>904</v>
       </c>
-      <c r="F292" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G292" s="28"/>
-      <c r="H292" s="28"/>
-      <c r="I292" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J292" s="12" t="s">
+      <c r="F293" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G293" s="28"/>
+      <c r="H293" s="28"/>
+      <c r="I293" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J293" s="12" t="s">
         <v>905</v>
       </c>
-      <c r="K292" s="28"/>
+      <c r="K293" s="28"/>
     </row>
   </sheetData>
-  <sortState ref="A1:G411">
-    <sortCondition ref="A1:A411"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G412">
+    <sortCondition ref="A1:A412"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating Change Log file and QuikEval_Daughter_Board_List for next release 1.3.0.
</commit_message>
<xml_diff>
--- a/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
+++ b/Documentation/QuikEval_Daughter_Board_List_sorted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSajikum\Documents\Linduino\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884AB2E7-4D6B-48AF-9203-405E2B3EEB83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB04FE02-D7CB-4ADC-9D4F-5A3DC8F5A04D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20760" yWindow="1686" windowWidth="4110" windowHeight="8652" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="919">
   <si>
     <t>Description</t>
   </si>
@@ -2777,6 +2777,15 @@
   </si>
   <si>
     <t>Michael Peters</t>
+  </si>
+  <si>
+    <t>LTC7841</t>
+  </si>
+  <si>
+    <t>PolyPhase Synchronous Boost Controller with PMBus Interface</t>
+  </si>
+  <si>
+    <t>DC2978A</t>
   </si>
 </sst>
 </file>
@@ -2918,7 +2927,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2985,6 +2994,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -3262,10 +3272,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A3:K293" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
-  <autoFilter ref="A3:K293" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K292">
-    <sortCondition ref="A3:A292"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A3:K294" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
+  <autoFilter ref="A3:K294" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K293">
+    <sortCondition ref="A3:A293"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Product" dataDxfId="10" dataCellStyle="Normal"/>
@@ -3609,7 +3619,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3620,27 +3630,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L293"/>
+  <dimension ref="A1:L294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" topLeftCell="F267" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K288" sqref="K288"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5859375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.68359375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="109" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1171875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1015625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.87890625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5859375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.89453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.17578125" style="1"/>
+    <col min="10" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="7" t="s">
         <v>492</v>
       </c>
@@ -3648,21 +3658,21 @@
         <v>518</v>
       </c>
       <c r="E1" s="14">
-        <f>(COUNTIF(I4:I293,"Done")/(COUNTA(A4:A293)-COUNTIF(H4:H293,"No")))</f>
-        <v>0.86554621848739499</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+        <f>(COUNTIF(I4:I294,"Done")/(COUNTA(A4:A294)-COUNTIF(H4:H294,"No")))</f>
+        <v>0.86610878661087864</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" s="8" t="s">
         <v>519</v>
       </c>
       <c r="E2" s="14">
-        <f>(COUNTIF(F4:F293,"Yes")+(COUNTIF(F4:F293,"General"))+(COUNTIF(F4:F293,"Family")))/(COUNTA(A4:A293)-COUNTIF(H4:H293,"No"))</f>
-        <v>0.96638655462184875</v>
+        <f>(COUNTIF(F4:F294,"Yes")+(COUNTIF(F4:F294,"General"))+(COUNTIF(F4:F294,"Family")))/(COUNTA(A4:A294)-COUNTIF(H4:H294,"No"))</f>
+        <v>0.96652719665271969</v>
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="5" t="s">
         <v>493</v>
       </c>
@@ -3697,7 +3707,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="13" t="s">
         <v>315</v>
       </c>
@@ -3720,7 +3730,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="13" t="s">
         <v>127</v>
       </c>
@@ -3743,7 +3753,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="12" t="s">
         <v>136</v>
       </c>
@@ -3766,7 +3776,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="12" t="s">
         <v>677</v>
       </c>
@@ -3795,7 +3805,7 @@
       </c>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="13" t="s">
         <v>370</v>
       </c>
@@ -3824,7 +3834,7 @@
       </c>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="12" t="s">
         <v>388</v>
       </c>
@@ -3853,7 +3863,7 @@
       </c>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A10" s="12" t="s">
         <v>428</v>
       </c>
@@ -3882,7 +3892,7 @@
       </c>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
@@ -3915,7 +3925,7 @@
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A12" s="12" t="s">
         <v>593</v>
       </c>
@@ -3936,7 +3946,7 @@
       </c>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A13" s="12" t="s">
         <v>348</v>
       </c>
@@ -3965,7 +3975,7 @@
       </c>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A14" s="12" t="s">
         <v>334</v>
       </c>
@@ -3994,7 +4004,7 @@
       </c>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15" s="12" t="s">
         <v>351</v>
       </c>
@@ -4023,7 +4033,7 @@
       </c>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A16" s="13" t="s">
         <v>285</v>
       </c>
@@ -4052,7 +4062,7 @@
       </c>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:11" s="27" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A17" s="12" t="s">
         <v>331</v>
       </c>
@@ -4081,7 +4091,7 @@
       </c>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A18" s="12" t="s">
         <v>783</v>
       </c>
@@ -4112,7 +4122,7 @@
       </c>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="12" t="s">
         <v>782</v>
       </c>
@@ -4143,7 +4153,7 @@
       </c>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A20" s="12" t="s">
         <v>781</v>
       </c>
@@ -4174,7 +4184,7 @@
       </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" s="26" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A21" s="12" t="s">
         <v>780</v>
       </c>
@@ -4205,7 +4215,7 @@
       </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
@@ -4236,7 +4246,7 @@
       </c>
       <c r="K22" s="13"/>
     </row>
-    <row r="23" spans="1:11" s="15" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23" s="13" t="s">
         <v>15</v>
       </c>
@@ -4265,7 +4275,7 @@
       </c>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A24" s="12" t="s">
         <v>880</v>
       </c>
@@ -4294,7 +4304,7 @@
       </c>
       <c r="K24" s="28"/>
     </row>
-    <row r="25" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A25" s="12" t="s">
         <v>881</v>
       </c>
@@ -4323,7 +4333,7 @@
       </c>
       <c r="K25" s="28"/>
     </row>
-    <row r="26" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A26" s="12" t="s">
         <v>579</v>
       </c>
@@ -4350,7 +4360,7 @@
       </c>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A27" s="12" t="s">
         <v>600</v>
       </c>
@@ -4379,7 +4389,7 @@
       </c>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A28" s="24" t="s">
         <v>590</v>
       </c>
@@ -4408,7 +4418,7 @@
       </c>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A29" s="24" t="s">
         <v>764</v>
       </c>
@@ -4439,7 +4449,7 @@
       </c>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A30" s="24" t="s">
         <v>767</v>
       </c>
@@ -4470,7 +4480,7 @@
       </c>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A31" s="12" t="s">
         <v>587</v>
       </c>
@@ -4501,7 +4511,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A32" s="25" t="s">
         <v>769</v>
       </c>
@@ -4532,7 +4542,7 @@
       </c>
       <c r="K32" s="25"/>
     </row>
-    <row r="33" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A33" s="24" t="s">
         <v>574</v>
       </c>
@@ -4561,7 +4571,7 @@
       </c>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A34" s="12" t="s">
         <v>892</v>
       </c>
@@ -4590,7 +4600,7 @@
       </c>
       <c r="K34" s="28"/>
     </row>
-    <row r="35" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A35" s="12" t="s">
         <v>893</v>
       </c>
@@ -4619,7 +4629,7 @@
       </c>
       <c r="K35" s="28"/>
     </row>
-    <row r="36" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A36" s="12" t="s">
         <v>886</v>
       </c>
@@ -4648,7 +4658,7 @@
       </c>
       <c r="K36" s="28"/>
     </row>
-    <row r="37" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A37" s="12" t="s">
         <v>887</v>
       </c>
@@ -4677,7 +4687,7 @@
       </c>
       <c r="K37" s="28"/>
     </row>
-    <row r="38" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A38" s="24" t="s">
         <v>875</v>
       </c>
@@ -4708,7 +4718,7 @@
       </c>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A39" s="24" t="s">
         <v>589</v>
       </c>
@@ -4739,7 +4749,7 @@
       </c>
       <c r="K39" s="24"/>
     </row>
-    <row r="40" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A40" s="12" t="s">
         <v>303</v>
       </c>
@@ -4770,7 +4780,7 @@
       </c>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A41" s="12" t="s">
         <v>300</v>
       </c>
@@ -4801,7 +4811,7 @@
       </c>
       <c r="K41" s="12"/>
     </row>
-    <row r="42" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A42" s="12" t="s">
         <v>297</v>
       </c>
@@ -4832,7 +4842,7 @@
       </c>
       <c r="K42" s="12"/>
     </row>
-    <row r="43" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A43" s="12" t="s">
         <v>53</v>
       </c>
@@ -4863,7 +4873,7 @@
       </c>
       <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A44" s="12" t="s">
         <v>53</v>
       </c>
@@ -4894,7 +4904,7 @@
       </c>
       <c r="K44" s="12"/>
     </row>
-    <row r="45" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A45" s="13" t="s">
         <v>41</v>
       </c>
@@ -4925,7 +4935,7 @@
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="46" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A46" s="13" t="s">
         <v>41</v>
       </c>
@@ -4956,7 +4966,7 @@
       </c>
       <c r="K46" s="13"/>
     </row>
-    <row r="47" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A47" s="12" t="s">
         <v>294</v>
       </c>
@@ -4987,7 +4997,7 @@
       </c>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A48" s="12" t="s">
         <v>291</v>
       </c>
@@ -5016,7 +5026,7 @@
       </c>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A49" s="12" t="s">
         <v>56</v>
       </c>
@@ -5047,7 +5057,7 @@
       </c>
       <c r="K49" s="12"/>
     </row>
-    <row r="50" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A50" s="12" t="s">
         <v>56</v>
       </c>
@@ -5078,7 +5088,7 @@
       </c>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A51" s="13" t="s">
         <v>44</v>
       </c>
@@ -5109,7 +5119,7 @@
       </c>
       <c r="K51" s="13"/>
     </row>
-    <row r="52" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A52" s="12" t="s">
         <v>44</v>
       </c>
@@ -5140,7 +5150,7 @@
       </c>
       <c r="K52" s="12"/>
     </row>
-    <row r="53" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A53" s="12" t="s">
         <v>62</v>
       </c>
@@ -5171,7 +5181,7 @@
       </c>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A54" s="12" t="s">
         <v>62</v>
       </c>
@@ -5202,7 +5212,7 @@
       </c>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A55" s="12" t="s">
         <v>47</v>
       </c>
@@ -5233,7 +5243,7 @@
       </c>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A56" s="12" t="s">
         <v>47</v>
       </c>
@@ -5264,7 +5274,7 @@
       </c>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A57" s="12" t="s">
         <v>581</v>
       </c>
@@ -5285,7 +5295,7 @@
       </c>
       <c r="K57" s="12"/>
     </row>
-    <row r="58" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="12" t="s">
         <v>50</v>
       </c>
@@ -5316,7 +5326,7 @@
       </c>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A59" s="13" t="s">
         <v>50</v>
       </c>
@@ -5347,7 +5357,7 @@
       </c>
       <c r="K59" s="13"/>
     </row>
-    <row r="60" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="12" t="s">
         <v>59</v>
       </c>
@@ -5376,7 +5386,7 @@
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A61" s="12" t="s">
         <v>59</v>
       </c>
@@ -5403,7 +5413,7 @@
       <c r="J61" s="13"/>
       <c r="K61" s="12"/>
     </row>
-    <row r="62" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A62" s="24" t="s">
         <v>836</v>
       </c>
@@ -5434,7 +5444,7 @@
       </c>
       <c r="K62" s="24"/>
     </row>
-    <row r="63" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A63" s="12" t="s">
         <v>850</v>
       </c>
@@ -5463,7 +5473,7 @@
       </c>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A64" s="24" t="s">
         <v>834</v>
       </c>
@@ -5494,7 +5504,7 @@
       </c>
       <c r="K64" s="24"/>
     </row>
-    <row r="65" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A65" s="12" t="s">
         <v>77</v>
       </c>
@@ -5523,7 +5533,7 @@
       </c>
       <c r="K65" s="12"/>
     </row>
-    <row r="66" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A66" s="12" t="s">
         <v>77</v>
       </c>
@@ -5552,7 +5562,7 @@
       </c>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A67" s="12" t="s">
         <v>65</v>
       </c>
@@ -5581,7 +5591,7 @@
       </c>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A68" s="12" t="s">
         <v>65</v>
       </c>
@@ -5610,7 +5620,7 @@
       </c>
       <c r="K68" s="12"/>
     </row>
-    <row r="69" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A69" s="21" t="s">
         <v>565</v>
       </c>
@@ -5641,7 +5651,7 @@
       </c>
       <c r="K69" s="22"/>
     </row>
-    <row r="70" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A70" s="13" t="s">
         <v>80</v>
       </c>
@@ -5670,7 +5680,7 @@
       </c>
       <c r="K70" s="13"/>
     </row>
-    <row r="71" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A71" s="13" t="s">
         <v>80</v>
       </c>
@@ -5699,7 +5709,7 @@
       </c>
       <c r="K71" s="13"/>
     </row>
-    <row r="72" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A72" s="12" t="s">
         <v>68</v>
       </c>
@@ -5728,7 +5738,7 @@
       </c>
       <c r="K72" s="12"/>
     </row>
-    <row r="73" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A73" s="13" t="s">
         <v>68</v>
       </c>
@@ -5757,7 +5767,7 @@
       </c>
       <c r="K73" s="13"/>
     </row>
-    <row r="74" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A74" s="12" t="s">
         <v>564</v>
       </c>
@@ -5788,7 +5798,7 @@
       </c>
       <c r="K74" s="12"/>
     </row>
-    <row r="75" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A75" s="12" t="s">
         <v>83</v>
       </c>
@@ -5819,7 +5829,7 @@
       </c>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A76" s="12" t="s">
         <v>83</v>
       </c>
@@ -5846,7 +5856,7 @@
       <c r="J76" s="22"/>
       <c r="K76" s="12"/>
     </row>
-    <row r="77" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A77" s="12" t="s">
         <v>71</v>
       </c>
@@ -5877,7 +5887,7 @@
       </c>
       <c r="K77" s="12"/>
     </row>
-    <row r="78" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A78" s="12" t="s">
         <v>71</v>
       </c>
@@ -5904,7 +5914,7 @@
       <c r="J78" s="22"/>
       <c r="K78" s="12"/>
     </row>
-    <row r="79" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A79" s="12" t="s">
         <v>10</v>
       </c>
@@ -5933,7 +5943,7 @@
       </c>
       <c r="K79" s="12"/>
     </row>
-    <row r="80" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A80" s="12" t="s">
         <v>10</v>
       </c>
@@ -5964,7 +5974,7 @@
       </c>
       <c r="K80" s="12"/>
     </row>
-    <row r="81" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A81" s="12" t="s">
         <v>74</v>
       </c>
@@ -5993,7 +6003,7 @@
       </c>
       <c r="K81" s="12"/>
     </row>
-    <row r="82" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A82" s="12" t="s">
         <v>74</v>
       </c>
@@ -6022,7 +6032,7 @@
       </c>
       <c r="K82" s="12"/>
     </row>
-    <row r="83" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A83" s="12" t="s">
         <v>86</v>
       </c>
@@ -6051,7 +6061,7 @@
       </c>
       <c r="K83" s="12"/>
     </row>
-    <row r="84" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A84" s="13" t="s">
         <v>86</v>
       </c>
@@ -6080,7 +6090,7 @@
       </c>
       <c r="K84" s="13"/>
     </row>
-    <row r="85" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A85" s="12" t="s">
         <v>582</v>
       </c>
@@ -6109,7 +6119,7 @@
       </c>
       <c r="K85" s="12"/>
     </row>
-    <row r="86" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A86" s="12" t="s">
         <v>183</v>
       </c>
@@ -6138,7 +6148,7 @@
       </c>
       <c r="K86" s="12"/>
     </row>
-    <row r="87" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A87" s="12" t="s">
         <v>186</v>
       </c>
@@ -6167,7 +6177,7 @@
       </c>
       <c r="K87" s="12"/>
     </row>
-    <row r="88" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A88" s="13" t="s">
         <v>189</v>
       </c>
@@ -6196,7 +6206,7 @@
       </c>
       <c r="K88" s="13"/>
     </row>
-    <row r="89" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A89" s="12" t="s">
         <v>572</v>
       </c>
@@ -6221,7 +6231,7 @@
       <c r="J89" s="13"/>
       <c r="K89" s="12"/>
     </row>
-    <row r="90" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A90" s="12" t="s">
         <v>373</v>
       </c>
@@ -6246,7 +6256,7 @@
       <c r="J90" s="13"/>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A91" s="12" t="s">
         <v>376</v>
       </c>
@@ -6271,7 +6281,7 @@
       <c r="J91" s="13"/>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A92" s="12" t="s">
         <v>397</v>
       </c>
@@ -6300,7 +6310,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A93" s="12" t="s">
         <v>634</v>
       </c>
@@ -6331,7 +6341,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A94" s="12" t="s">
         <v>637</v>
       </c>
@@ -6362,7 +6372,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A95" s="12" t="s">
         <v>367</v>
       </c>
@@ -6391,7 +6401,7 @@
       </c>
       <c r="K95" s="12"/>
     </row>
-    <row r="96" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A96" s="12" t="s">
         <v>382</v>
       </c>
@@ -6416,7 +6426,7 @@
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A97" s="12" t="s">
         <v>394</v>
       </c>
@@ -6441,7 +6451,7 @@
       <c r="J97" s="13"/>
       <c r="K97" s="12"/>
     </row>
-    <row r="98" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A98" s="12" t="s">
         <v>204</v>
       </c>
@@ -6466,7 +6476,7 @@
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
     </row>
-    <row r="99" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A99" s="12" t="s">
         <v>204</v>
       </c>
@@ -6489,7 +6499,7 @@
       <c r="J99" s="13"/>
       <c r="K99" s="12"/>
     </row>
-    <row r="100" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A100" s="12" t="s">
         <v>364</v>
       </c>
@@ -6518,7 +6528,7 @@
       </c>
       <c r="K100" s="12"/>
     </row>
-    <row r="101" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A101" s="13" t="s">
         <v>483</v>
       </c>
@@ -6547,7 +6557,7 @@
       </c>
       <c r="K101" s="13"/>
     </row>
-    <row r="102" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A102" s="12" t="s">
         <v>446</v>
       </c>
@@ -6570,7 +6580,7 @@
       <c r="J102" s="12"/>
       <c r="K102" s="12"/>
     </row>
-    <row r="103" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A103" s="12" t="s">
         <v>443</v>
       </c>
@@ -6593,7 +6603,7 @@
       <c r="J103" s="12"/>
       <c r="K103" s="12"/>
     </row>
-    <row r="104" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A104" s="12" t="s">
         <v>440</v>
       </c>
@@ -6622,7 +6632,7 @@
       </c>
       <c r="K104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A105" s="12" t="s">
         <v>391</v>
       </c>
@@ -6651,7 +6661,7 @@
       </c>
       <c r="K105" s="12"/>
     </row>
-    <row r="106" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A106" s="12" t="s">
         <v>391</v>
       </c>
@@ -6680,7 +6690,7 @@
       </c>
       <c r="K106" s="12"/>
     </row>
-    <row r="107" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A107" s="12" t="s">
         <v>258</v>
       </c>
@@ -6705,7 +6715,7 @@
       <c r="J107" s="13"/>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A108" s="12" t="s">
         <v>261</v>
       </c>
@@ -6730,7 +6740,7 @@
       <c r="J108" s="13"/>
       <c r="K108" s="12"/>
     </row>
-    <row r="109" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A109" s="12" t="s">
         <v>337</v>
       </c>
@@ -6755,7 +6765,7 @@
       <c r="J109" s="12"/>
       <c r="K109" s="12"/>
     </row>
-    <row r="110" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A110" s="12" t="s">
         <v>340</v>
       </c>
@@ -6780,7 +6790,7 @@
       <c r="J110" s="13"/>
       <c r="K110" s="12"/>
     </row>
-    <row r="111" spans="1:11" s="26" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:11" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A111" s="13" t="s">
         <v>325</v>
       </c>
@@ -6807,7 +6817,7 @@
       <c r="J111" s="13"/>
       <c r="K111" s="13"/>
     </row>
-    <row r="112" spans="1:11" s="26" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:11" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A112" s="12" t="s">
         <v>180</v>
       </c>
@@ -6836,7 +6846,7 @@
       </c>
       <c r="K112" s="12"/>
     </row>
-    <row r="113" spans="1:11" s="26" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:11" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A113" s="12" t="s">
         <v>195</v>
       </c>
@@ -6865,7 +6875,7 @@
       </c>
       <c r="K113" s="12"/>
     </row>
-    <row r="114" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A114" s="12" t="s">
         <v>358</v>
       </c>
@@ -6890,7 +6900,7 @@
       <c r="J114" s="12"/>
       <c r="K114" s="12"/>
     </row>
-    <row r="115" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A115" s="12" t="s">
         <v>489</v>
       </c>
@@ -6917,7 +6927,7 @@
       <c r="J115" s="12"/>
       <c r="K115" s="12"/>
     </row>
-    <row r="116" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A116" s="12" t="s">
         <v>171</v>
       </c>
@@ -6942,7 +6952,7 @@
       <c r="J116" s="12"/>
       <c r="K116" s="12"/>
     </row>
-    <row r="117" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A117" s="12" t="s">
         <v>161</v>
       </c>
@@ -6967,7 +6977,7 @@
       <c r="J117" s="12"/>
       <c r="K117" s="12"/>
     </row>
-    <row r="118" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A118" s="12" t="s">
         <v>168</v>
       </c>
@@ -6992,7 +7002,7 @@
       <c r="J118" s="12"/>
       <c r="K118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A119" s="13" t="s">
         <v>158</v>
       </c>
@@ -7021,7 +7031,7 @@
       </c>
       <c r="K119" s="13"/>
     </row>
-    <row r="120" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A120" s="12" t="s">
         <v>425</v>
       </c>
@@ -7050,7 +7060,7 @@
       </c>
       <c r="K120" s="12"/>
     </row>
-    <row r="121" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A121" s="12" t="s">
         <v>475</v>
       </c>
@@ -7075,7 +7085,7 @@
       <c r="J121" s="12"/>
       <c r="K121" s="12"/>
     </row>
-    <row r="122" spans="1:11" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:11" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A122" s="12" t="s">
         <v>472</v>
       </c>
@@ -7104,7 +7114,7 @@
       </c>
       <c r="K122" s="12"/>
     </row>
-    <row r="123" spans="1:11" s="26" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:11" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A123" s="12" t="s">
         <v>478</v>
       </c>
@@ -7129,7 +7139,7 @@
       <c r="J123" s="12"/>
       <c r="K123" s="12"/>
     </row>
-    <row r="124" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A124" s="12" t="s">
         <v>469</v>
       </c>
@@ -7158,7 +7168,7 @@
       </c>
       <c r="K124" s="12"/>
     </row>
-    <row r="125" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A125" s="12" t="s">
         <v>481</v>
       </c>
@@ -7183,7 +7193,7 @@
       <c r="J125" s="12"/>
       <c r="K125" s="12"/>
     </row>
-    <row r="126" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A126" s="12" t="s">
         <v>218</v>
       </c>
@@ -7208,7 +7218,7 @@
       <c r="J126" s="12"/>
       <c r="K126" s="12"/>
     </row>
-    <row r="127" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A127" s="12" t="s">
         <v>227</v>
       </c>
@@ -7233,7 +7243,7 @@
       <c r="J127" s="12"/>
       <c r="K127" s="12"/>
     </row>
-    <row r="128" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A128" s="12" t="s">
         <v>215</v>
       </c>
@@ -7258,7 +7268,7 @@
       <c r="J128" s="12"/>
       <c r="K128" s="12"/>
     </row>
-    <row r="129" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A129" s="12" t="s">
         <v>224</v>
       </c>
@@ -7283,7 +7293,7 @@
       <c r="J129" s="12"/>
       <c r="K129" s="12"/>
     </row>
-    <row r="130" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A130" s="13" t="s">
         <v>212</v>
       </c>
@@ -7312,7 +7322,7 @@
       </c>
       <c r="K130" s="13"/>
     </row>
-    <row r="131" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A131" s="12" t="s">
         <v>221</v>
       </c>
@@ -7337,7 +7347,7 @@
       <c r="J131" s="12"/>
       <c r="K131" s="12"/>
     </row>
-    <row r="132" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A132" s="12" t="s">
         <v>235</v>
       </c>
@@ -7362,7 +7372,7 @@
       <c r="J132" s="12"/>
       <c r="K132" s="12"/>
     </row>
-    <row r="133" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A133" s="12" t="s">
         <v>244</v>
       </c>
@@ -7387,7 +7397,7 @@
       <c r="J133" s="12"/>
       <c r="K133" s="12"/>
     </row>
-    <row r="134" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A134" s="12" t="s">
         <v>232</v>
       </c>
@@ -7416,7 +7426,7 @@
       </c>
       <c r="K134" s="12"/>
     </row>
-    <row r="135" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A135" s="12" t="s">
         <v>241</v>
       </c>
@@ -7445,7 +7455,7 @@
       </c>
       <c r="K135" s="12"/>
     </row>
-    <row r="136" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A136" s="13" t="s">
         <v>230</v>
       </c>
@@ -7474,7 +7484,7 @@
       </c>
       <c r="K136" s="13"/>
     </row>
-    <row r="137" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A137" s="12" t="s">
         <v>230</v>
       </c>
@@ -7503,7 +7513,7 @@
       </c>
       <c r="K137" s="12"/>
     </row>
-    <row r="138" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A138" s="12" t="s">
         <v>238</v>
       </c>
@@ -7532,7 +7542,7 @@
       </c>
       <c r="K138" s="12"/>
     </row>
-    <row r="139" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A139" s="12" t="s">
         <v>583</v>
       </c>
@@ -7553,7 +7563,7 @@
       </c>
       <c r="K139" s="12"/>
     </row>
-    <row r="140" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A140" s="12" t="s">
         <v>814</v>
       </c>
@@ -7584,7 +7594,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="141" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A141" s="12" t="s">
         <v>584</v>
       </c>
@@ -7615,7 +7625,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="142" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A142" s="12" t="s">
         <v>379</v>
       </c>
@@ -7644,7 +7654,7 @@
       </c>
       <c r="K142" s="12"/>
     </row>
-    <row r="143" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A143" s="12" t="s">
         <v>414</v>
       </c>
@@ -7669,7 +7679,7 @@
       <c r="J143" s="12"/>
       <c r="K143" s="12"/>
     </row>
-    <row r="144" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A144" s="12" t="s">
         <v>417</v>
       </c>
@@ -7694,7 +7704,7 @@
       <c r="J144" s="12"/>
       <c r="K144" s="12"/>
     </row>
-    <row r="145" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A145" s="12" t="s">
         <v>431</v>
       </c>
@@ -7723,7 +7733,7 @@
       </c>
       <c r="K145" s="12"/>
     </row>
-    <row r="146" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A146" s="12" t="s">
         <v>463</v>
       </c>
@@ -7752,7 +7762,7 @@
       </c>
       <c r="K146" s="12"/>
     </row>
-    <row r="147" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A147" s="24" t="s">
         <v>434</v>
       </c>
@@ -7781,7 +7791,7 @@
       <c r="J147" s="25"/>
       <c r="K147" s="24"/>
     </row>
-    <row r="148" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A148" s="24" t="s">
         <v>460</v>
       </c>
@@ -7810,7 +7820,7 @@
       </c>
       <c r="K148" s="24"/>
     </row>
-    <row r="149" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A149" s="24" t="s">
         <v>466</v>
       </c>
@@ -7839,7 +7849,7 @@
       <c r="J149" s="25"/>
       <c r="K149" s="24"/>
     </row>
-    <row r="150" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A150" s="25" t="s">
         <v>269</v>
       </c>
@@ -7868,7 +7878,7 @@
       <c r="J150" s="25"/>
       <c r="K150" s="25"/>
     </row>
-    <row r="151" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A151" s="24" t="s">
         <v>326</v>
       </c>
@@ -7895,7 +7905,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="152" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A152" s="24" t="s">
         <v>355</v>
       </c>
@@ -7928,7 +7938,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="153" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A153" s="25" t="s">
         <v>175</v>
       </c>
@@ -7961,7 +7971,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="154" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A154" s="24" t="s">
         <v>352</v>
       </c>
@@ -7992,7 +8002,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="155" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A155" s="24" t="s">
         <v>201</v>
       </c>
@@ -8023,7 +8033,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="156" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A156" s="24" t="s">
         <v>328</v>
       </c>
@@ -8052,7 +8062,7 @@
       </c>
       <c r="K156" s="24"/>
     </row>
-    <row r="157" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A157" s="12" t="s">
         <v>270</v>
       </c>
@@ -8085,7 +8095,7 @@
       </c>
       <c r="K157" s="12"/>
     </row>
-    <row r="158" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A158" s="12" t="s">
         <v>32</v>
       </c>
@@ -8114,7 +8124,7 @@
       </c>
       <c r="K158" s="12"/>
     </row>
-    <row r="159" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A159" s="13" t="s">
         <v>604</v>
       </c>
@@ -8143,7 +8153,7 @@
       </c>
       <c r="K159" s="13"/>
     </row>
-    <row r="160" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A160" s="13" t="s">
         <v>153</v>
       </c>
@@ -8172,7 +8182,7 @@
       </c>
       <c r="K160" s="13"/>
     </row>
-    <row r="161" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A161" s="13" t="s">
         <v>131</v>
       </c>
@@ -8201,7 +8211,7 @@
       </c>
       <c r="K161" s="13"/>
     </row>
-    <row r="162" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A162" s="12" t="s">
         <v>208</v>
       </c>
@@ -8230,7 +8240,7 @@
       </c>
       <c r="K162" s="12"/>
     </row>
-    <row r="163" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A163" s="12" t="s">
         <v>192</v>
       </c>
@@ -8259,7 +8269,7 @@
       </c>
       <c r="K163" s="12"/>
     </row>
-    <row r="164" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A164" s="12" t="s">
         <v>838</v>
       </c>
@@ -8288,7 +8298,7 @@
       </c>
       <c r="K164" s="28"/>
     </row>
-    <row r="165" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A165" s="12" t="s">
         <v>726</v>
       </c>
@@ -8317,7 +8327,7 @@
       </c>
       <c r="K165" s="12"/>
     </row>
-    <row r="166" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A166" s="13" t="s">
         <v>532</v>
       </c>
@@ -8346,7 +8356,7 @@
       </c>
       <c r="K166" s="13"/>
     </row>
-    <row r="167" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A167" s="13" t="s">
         <v>513</v>
       </c>
@@ -8375,7 +8385,7 @@
       </c>
       <c r="K167" s="13"/>
     </row>
-    <row r="168" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A168" s="12" t="s">
         <v>403</v>
       </c>
@@ -8400,7 +8410,7 @@
       <c r="J168" s="13"/>
       <c r="K168" s="12"/>
     </row>
-    <row r="169" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A169" s="13" t="s">
         <v>273</v>
       </c>
@@ -8427,7 +8437,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="170" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A170" s="13" t="s">
         <v>150</v>
       </c>
@@ -8456,7 +8466,7 @@
       </c>
       <c r="K170" s="13"/>
     </row>
-    <row r="171" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A171" s="13" t="s">
         <v>276</v>
       </c>
@@ -8483,7 +8493,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="172" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A172" s="12" t="s">
         <v>361</v>
       </c>
@@ -8508,7 +8518,7 @@
       <c r="J172" s="12"/>
       <c r="K172" s="12"/>
     </row>
-    <row r="173" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A173" s="12" t="s">
         <v>279</v>
       </c>
@@ -8535,7 +8545,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="174" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A174" s="12" t="s">
         <v>139</v>
       </c>
@@ -8560,7 +8570,7 @@
       <c r="J174" s="12"/>
       <c r="K174" s="12"/>
     </row>
-    <row r="175" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A175" s="12" t="s">
         <v>198</v>
       </c>
@@ -8587,7 +8597,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="176" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A176" s="13" t="s">
         <v>147</v>
       </c>
@@ -8616,7 +8626,7 @@
       </c>
       <c r="K176" s="13"/>
     </row>
-    <row r="177" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A177" s="13" t="s">
         <v>643</v>
       </c>
@@ -8643,7 +8653,7 @@
       </c>
       <c r="K177" s="13"/>
     </row>
-    <row r="178" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A178" s="12" t="s">
         <v>609</v>
       </c>
@@ -8672,7 +8682,7 @@
       </c>
       <c r="K178" s="12"/>
     </row>
-    <row r="179" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A179" s="12" t="s">
         <v>625</v>
       </c>
@@ -8701,7 +8711,7 @@
       </c>
       <c r="K179" s="12"/>
     </row>
-    <row r="180" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A180" s="13" t="s">
         <v>626</v>
       </c>
@@ -8730,7 +8740,7 @@
       </c>
       <c r="K180" s="13"/>
     </row>
-    <row r="181" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A181" s="12" t="s">
         <v>651</v>
       </c>
@@ -8759,7 +8769,7 @@
       </c>
       <c r="K181" s="12"/>
     </row>
-    <row r="182" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A182" s="13" t="s">
         <v>13</v>
       </c>
@@ -8790,7 +8800,7 @@
       </c>
       <c r="K182" s="25"/>
     </row>
-    <row r="183" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A183" s="12" t="s">
         <v>606</v>
       </c>
@@ -8823,7 +8833,7 @@
       </c>
       <c r="K183" s="24"/>
     </row>
-    <row r="184" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A184" s="12" t="s">
         <v>35</v>
       </c>
@@ -8852,7 +8862,7 @@
       </c>
       <c r="K184" s="12"/>
     </row>
-    <row r="185" spans="1:11" s="19" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:11" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A185" s="12" t="s">
         <v>607</v>
       </c>
@@ -8883,7 +8893,7 @@
       </c>
       <c r="K185" s="24"/>
     </row>
-    <row r="186" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A186" s="12" t="s">
         <v>730</v>
       </c>
@@ -8912,7 +8922,7 @@
       </c>
       <c r="K186" s="12"/>
     </row>
-    <row r="187" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A187" s="12" t="s">
         <v>797</v>
       </c>
@@ -8943,7 +8953,7 @@
       </c>
       <c r="K187" s="12"/>
     </row>
-    <row r="188" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A188" s="12" t="s">
         <v>554</v>
       </c>
@@ -8972,7 +8982,7 @@
       </c>
       <c r="K188" s="12"/>
     </row>
-    <row r="189" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A189" s="12" t="s">
         <v>22</v>
       </c>
@@ -9001,7 +9011,7 @@
       </c>
       <c r="K189" s="12"/>
     </row>
-    <row r="190" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A190" s="12" t="s">
         <v>522</v>
       </c>
@@ -9030,7 +9040,7 @@
       </c>
       <c r="K190" s="12"/>
     </row>
-    <row r="191" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A191" s="25" t="s">
         <v>577</v>
       </c>
@@ -9059,7 +9069,7 @@
       </c>
       <c r="K191" s="25"/>
     </row>
-    <row r="192" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A192" s="24" t="s">
         <v>577</v>
       </c>
@@ -9088,7 +9098,7 @@
       </c>
       <c r="K192" s="24"/>
     </row>
-    <row r="193" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A193" s="24" t="s">
         <v>588</v>
       </c>
@@ -9113,7 +9123,7 @@
       </c>
       <c r="K193" s="24"/>
     </row>
-    <row r="194" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A194" s="24" t="s">
         <v>317</v>
       </c>
@@ -9144,7 +9154,7 @@
       </c>
       <c r="K194" s="24"/>
     </row>
-    <row r="195" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A195" s="12" t="s">
         <v>317</v>
       </c>
@@ -9173,7 +9183,7 @@
       </c>
       <c r="K195" s="12"/>
     </row>
-    <row r="196" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A196" s="12" t="s">
         <v>913</v>
       </c>
@@ -9202,7 +9212,7 @@
       </c>
       <c r="K196" s="12"/>
     </row>
-    <row r="197" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A197" s="12" t="s">
         <v>872</v>
       </c>
@@ -9227,7 +9237,7 @@
       </c>
       <c r="K197" s="28"/>
     </row>
-    <row r="198" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A198" s="12" t="s">
         <v>736</v>
       </c>
@@ -9256,7 +9266,7 @@
       </c>
       <c r="K198" s="12"/>
     </row>
-    <row r="199" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A199" s="12" t="s">
         <v>631</v>
       </c>
@@ -9285,7 +9295,7 @@
       </c>
       <c r="K199" s="12"/>
     </row>
-    <row r="200" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A200" s="12" t="s">
         <v>631</v>
       </c>
@@ -9314,7 +9324,7 @@
       </c>
       <c r="K200" s="12"/>
     </row>
-    <row r="201" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A201" s="12" t="s">
         <v>667</v>
       </c>
@@ -9343,7 +9353,7 @@
       </c>
       <c r="K201" s="12"/>
     </row>
-    <row r="202" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A202" s="12" t="s">
         <v>738</v>
       </c>
@@ -9374,7 +9384,7 @@
       </c>
       <c r="K202" s="12"/>
     </row>
-    <row r="203" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A203" s="12" t="s">
         <v>670</v>
       </c>
@@ -9403,7 +9413,7 @@
       </c>
       <c r="K203" s="12"/>
     </row>
-    <row r="204" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A204" s="12" t="s">
         <v>566</v>
       </c>
@@ -9432,7 +9442,7 @@
       </c>
       <c r="K204" s="12"/>
     </row>
-    <row r="205" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A205" s="12" t="s">
         <v>580</v>
       </c>
@@ -9461,7 +9471,7 @@
       </c>
       <c r="K205" s="12"/>
     </row>
-    <row r="206" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A206" s="12" t="s">
         <v>748</v>
       </c>
@@ -9490,7 +9500,7 @@
       </c>
       <c r="K206" s="12"/>
     </row>
-    <row r="207" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A207" s="12" t="s">
         <v>28</v>
       </c>
@@ -9519,7 +9529,7 @@
       </c>
       <c r="K207" s="12"/>
     </row>
-    <row r="208" spans="1:11" s="11" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:11" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A208" s="13" t="s">
         <v>130</v>
       </c>
@@ -9548,7 +9558,7 @@
       </c>
       <c r="K208" s="13"/>
     </row>
-    <row r="209" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A209" s="12" t="s">
         <v>841</v>
       </c>
@@ -9577,7 +9587,7 @@
       </c>
       <c r="K209" s="28"/>
     </row>
-    <row r="210" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A210" s="13" t="s">
         <v>385</v>
       </c>
@@ -9600,7 +9610,7 @@
       <c r="J210" s="13"/>
       <c r="K210" s="13"/>
     </row>
-    <row r="211" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A211" s="12" t="s">
         <v>400</v>
       </c>
@@ -9623,7 +9633,7 @@
       <c r="J211" s="12"/>
       <c r="K211" s="12"/>
     </row>
-    <row r="212" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A212" s="12" t="s">
         <v>250</v>
       </c>
@@ -9646,7 +9656,7 @@
       <c r="J212" s="12"/>
       <c r="K212" s="12"/>
     </row>
-    <row r="213" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A213" s="12" t="s">
         <v>250</v>
       </c>
@@ -9669,7 +9679,7 @@
       <c r="J213" s="12"/>
       <c r="K213" s="12"/>
     </row>
-    <row r="214" spans="1:11" s="10" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:11" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A214" s="12" t="s">
         <v>437</v>
       </c>
@@ -9692,7 +9702,7 @@
       <c r="J214" s="12"/>
       <c r="K214" s="12"/>
     </row>
-    <row r="215" spans="1:11" s="9" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A215" s="12" t="s">
         <v>452</v>
       </c>
@@ -9715,7 +9725,7 @@
       <c r="J215" s="12"/>
       <c r="K215" s="12"/>
     </row>
-    <row r="216" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A216" s="12" t="s">
         <v>452</v>
       </c>
@@ -9738,7 +9748,7 @@
       <c r="J216" s="12"/>
       <c r="K216" s="12"/>
     </row>
-    <row r="217" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A217" s="12" t="s">
         <v>457</v>
       </c>
@@ -9761,7 +9771,7 @@
       <c r="J217" s="12"/>
       <c r="K217" s="12"/>
     </row>
-    <row r="218" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A218" s="12" t="s">
         <v>247</v>
       </c>
@@ -9784,7 +9794,7 @@
       <c r="J218" s="12"/>
       <c r="K218" s="12"/>
     </row>
-    <row r="219" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A219" s="12" t="s">
         <v>264</v>
       </c>
@@ -9807,7 +9817,7 @@
       <c r="J219" s="12"/>
       <c r="K219" s="12"/>
     </row>
-    <row r="220" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A220" s="12" t="s">
         <v>264</v>
       </c>
@@ -9830,7 +9840,7 @@
       <c r="J220" s="12"/>
       <c r="K220" s="12"/>
     </row>
-    <row r="221" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A221" s="13" t="s">
         <v>288</v>
       </c>
@@ -9853,7 +9863,7 @@
       <c r="J221" s="13"/>
       <c r="K221" s="13"/>
     </row>
-    <row r="222" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A222" s="12" t="s">
         <v>255</v>
       </c>
@@ -9876,7 +9886,7 @@
       <c r="J222" s="12"/>
       <c r="K222" s="12"/>
     </row>
-    <row r="223" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A223" s="13" t="s">
         <v>320</v>
       </c>
@@ -9899,7 +9909,7 @@
       <c r="J223" s="13"/>
       <c r="K223" s="13"/>
     </row>
-    <row r="224" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A224" s="13" t="s">
         <v>320</v>
       </c>
@@ -9922,7 +9932,7 @@
       <c r="J224" s="13"/>
       <c r="K224" s="13"/>
     </row>
-    <row r="225" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A225" s="12" t="s">
         <v>309</v>
       </c>
@@ -9945,7 +9955,7 @@
       <c r="J225" s="12"/>
       <c r="K225" s="12"/>
     </row>
-    <row r="226" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A226" s="12" t="s">
         <v>679</v>
       </c>
@@ -9974,7 +9984,7 @@
       </c>
       <c r="K226" s="12"/>
     </row>
-    <row r="227" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A227" s="12" t="s">
         <v>683</v>
       </c>
@@ -10001,7 +10011,7 @@
       </c>
       <c r="K227" s="12"/>
     </row>
-    <row r="228" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A228" s="12" t="s">
         <v>19</v>
       </c>
@@ -10024,7 +10034,7 @@
       <c r="J228" s="12"/>
       <c r="K228" s="12"/>
     </row>
-    <row r="229" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A229" s="12" t="s">
         <v>29</v>
       </c>
@@ -10055,7 +10065,7 @@
       </c>
       <c r="K229" s="12"/>
     </row>
-    <row r="230" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A230" s="12" t="s">
         <v>29</v>
       </c>
@@ -10084,7 +10094,7 @@
       </c>
       <c r="K230" s="12"/>
     </row>
-    <row r="231" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A231" s="12" t="s">
         <v>174</v>
       </c>
@@ -10107,7 +10117,7 @@
       <c r="J231" s="12"/>
       <c r="K231" s="12"/>
     </row>
-    <row r="232" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A232" s="12" t="s">
         <v>511</v>
       </c>
@@ -10134,7 +10144,7 @@
       <c r="J232" s="12"/>
       <c r="K232" s="12"/>
     </row>
-    <row r="233" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A233" s="12" t="s">
         <v>534</v>
       </c>
@@ -10163,7 +10173,7 @@
       </c>
       <c r="K233" s="12"/>
     </row>
-    <row r="234" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:11" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A234" s="12" t="s">
         <v>535</v>
       </c>
@@ -10192,7 +10202,7 @@
       </c>
       <c r="K234" s="12"/>
     </row>
-    <row r="235" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A235" s="13" t="s">
         <v>536</v>
       </c>
@@ -10221,7 +10231,7 @@
       </c>
       <c r="K235" s="13"/>
     </row>
-    <row r="236" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A236" s="12" t="s">
         <v>865</v>
       </c>
@@ -10248,7 +10258,7 @@
       <c r="J236" s="28"/>
       <c r="K236" s="28"/>
     </row>
-    <row r="237" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A237" s="12" t="s">
         <v>693</v>
       </c>
@@ -10277,7 +10287,7 @@
       </c>
       <c r="K237" s="12"/>
     </row>
-    <row r="238" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A238" s="12" t="s">
         <v>346</v>
       </c>
@@ -10302,7 +10312,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="239" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:11" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A239" s="12" t="s">
         <v>406</v>
       </c>
@@ -10325,7 +10335,7 @@
       <c r="J239" s="12"/>
       <c r="K239" s="12"/>
     </row>
-    <row r="240" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A240" s="12" t="s">
         <v>306</v>
       </c>
@@ -10354,7 +10364,7 @@
       </c>
       <c r="K240" s="12"/>
     </row>
-    <row r="241" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A241" s="12" t="s">
         <v>108</v>
       </c>
@@ -10383,7 +10393,7 @@
       </c>
       <c r="K241" s="12"/>
     </row>
-    <row r="242" spans="1:11" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:11" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A242" s="12" t="s">
         <v>103</v>
       </c>
@@ -10406,7 +10416,7 @@
       <c r="J242" s="12"/>
       <c r="K242" s="12"/>
     </row>
-    <row r="243" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A243" s="12" t="s">
         <v>449</v>
       </c>
@@ -10435,7 +10445,7 @@
       </c>
       <c r="K243" s="12"/>
     </row>
-    <row r="244" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A244" s="12" t="s">
         <v>312</v>
       </c>
@@ -10460,7 +10470,7 @@
       <c r="J244" s="12"/>
       <c r="K244" s="12"/>
     </row>
-    <row r="245" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A245" s="12" t="s">
         <v>282</v>
       </c>
@@ -10483,7 +10493,7 @@
       <c r="J245" s="12"/>
       <c r="K245" s="12"/>
     </row>
-    <row r="246" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A246" s="12" t="s">
         <v>207</v>
       </c>
@@ -10512,7 +10522,7 @@
       </c>
       <c r="K246" s="12"/>
     </row>
-    <row r="247" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A247" s="12" t="s">
         <v>420</v>
       </c>
@@ -10541,7 +10551,7 @@
       </c>
       <c r="K247" s="12"/>
     </row>
-    <row r="248" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A248" s="12" t="s">
         <v>486</v>
       </c>
@@ -10570,7 +10580,7 @@
       </c>
       <c r="K248" s="12"/>
     </row>
-    <row r="249" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A249" s="13" t="s">
         <v>144</v>
       </c>
@@ -10599,7 +10609,7 @@
       </c>
       <c r="K249" s="13"/>
     </row>
-    <row r="250" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A250" s="12" t="s">
         <v>558</v>
       </c>
@@ -10626,7 +10636,7 @@
       </c>
       <c r="K250" s="12"/>
     </row>
-    <row r="251" spans="1:11" s="15" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:11" s="15" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A251" s="12" t="s">
         <v>560</v>
       </c>
@@ -10655,7 +10665,7 @@
       </c>
       <c r="K251" s="12"/>
     </row>
-    <row r="252" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A252" s="13" t="s">
         <v>592</v>
       </c>
@@ -10682,7 +10692,7 @@
       </c>
       <c r="K252" s="13"/>
     </row>
-    <row r="253" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A253" s="12" t="s">
         <v>591</v>
       </c>
@@ -10709,7 +10719,7 @@
       </c>
       <c r="K253" s="12"/>
     </row>
-    <row r="254" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:11" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A254" s="12" t="s">
         <v>409</v>
       </c>
@@ -10732,7 +10742,7 @@
       <c r="J254" s="12"/>
       <c r="K254" s="12"/>
     </row>
-    <row r="255" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A255" s="12" t="s">
         <v>409</v>
       </c>
@@ -10755,7 +10765,7 @@
       <c r="J255" s="12"/>
       <c r="K255" s="12"/>
     </row>
-    <row r="256" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:11" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A256" s="12" t="s">
         <v>562</v>
       </c>
@@ -10782,7 +10792,7 @@
       </c>
       <c r="K256" s="12"/>
     </row>
-    <row r="257" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A257" s="24" t="s">
         <v>687</v>
       </c>
@@ -10809,7 +10819,7 @@
       </c>
       <c r="K257" s="24"/>
     </row>
-    <row r="258" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A258" s="12" t="s">
         <v>898</v>
       </c>
@@ -10836,7 +10846,7 @@
       </c>
       <c r="K258" s="28"/>
     </row>
-    <row r="259" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A259" s="24" t="s">
         <v>688</v>
       </c>
@@ -10865,7 +10875,7 @@
       </c>
       <c r="K259" s="24"/>
     </row>
-    <row r="260" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A260" s="24" t="s">
         <v>544</v>
       </c>
@@ -10894,7 +10904,7 @@
       </c>
       <c r="K260" s="24"/>
     </row>
-    <row r="261" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A261" s="24" t="s">
         <v>598</v>
       </c>
@@ -10919,7 +10929,7 @@
       </c>
       <c r="K261" s="24"/>
     </row>
-    <row r="262" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A262" s="24" t="s">
         <v>526</v>
       </c>
@@ -10948,7 +10958,7 @@
       </c>
       <c r="K262" s="24"/>
     </row>
-    <row r="263" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A263" s="24" t="s">
         <v>642</v>
       </c>
@@ -10975,7 +10985,7 @@
       </c>
       <c r="K263" s="24"/>
     </row>
-    <row r="264" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A264" s="24" t="s">
         <v>211</v>
       </c>
@@ -10998,7 +11008,7 @@
       <c r="J264" s="24"/>
       <c r="K264" s="24"/>
     </row>
-    <row r="265" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A265" s="24" t="s">
         <v>343</v>
       </c>
@@ -11021,7 +11031,7 @@
       <c r="J265" s="24"/>
       <c r="K265" s="24"/>
     </row>
-    <row r="266" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:12" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A266" s="24" t="s">
         <v>621</v>
       </c>
@@ -11048,7 +11058,7 @@
       </c>
       <c r="K266" s="24"/>
     </row>
-    <row r="267" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A267" s="24" t="s">
         <v>622</v>
       </c>
@@ -11075,7 +11085,7 @@
       </c>
       <c r="K267" s="24"/>
     </row>
-    <row r="268" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A268" s="24" t="s">
         <v>623</v>
       </c>
@@ -11098,7 +11108,7 @@
       <c r="J268" s="24"/>
       <c r="K268" s="24"/>
     </row>
-    <row r="269" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A269" s="24" t="s">
         <v>624</v>
       </c>
@@ -11121,7 +11131,7 @@
       <c r="J269" s="24"/>
       <c r="K269" s="24"/>
     </row>
-    <row r="270" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A270" s="24" t="s">
         <v>503</v>
       </c>
@@ -11148,7 +11158,7 @@
       </c>
       <c r="K270" s="24"/>
     </row>
-    <row r="271" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:12" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A271" s="24" t="s">
         <v>506</v>
       </c>
@@ -11175,7 +11185,7 @@
       </c>
       <c r="K271" s="24"/>
     </row>
-    <row r="272" spans="1:12" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:12" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A272" s="12" t="s">
         <v>906</v>
       </c>
@@ -11203,7 +11213,7 @@
       <c r="K272" s="28"/>
       <c r="L272" s="19"/>
     </row>
-    <row r="273" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A273" s="24" t="s">
         <v>804</v>
       </c>
@@ -11230,7 +11240,7 @@
       </c>
       <c r="K273" s="24"/>
     </row>
-    <row r="274" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A274" s="12" t="s">
         <v>907</v>
       </c>
@@ -11257,7 +11267,7 @@
       </c>
       <c r="K274" s="28"/>
     </row>
-    <row r="275" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A275" s="12" t="s">
         <v>908</v>
       </c>
@@ -11282,7 +11292,7 @@
       </c>
       <c r="K275" s="28"/>
     </row>
-    <row r="276" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A276" s="24" t="s">
         <v>25</v>
       </c>
@@ -11305,7 +11315,7 @@
       <c r="J276" s="24"/>
       <c r="K276" s="24"/>
     </row>
-    <row r="277" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A277" s="24" t="s">
         <v>509</v>
       </c>
@@ -11334,7 +11344,7 @@
       </c>
       <c r="K277" s="24"/>
     </row>
-    <row r="278" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A278" s="24" t="s">
         <v>507</v>
       </c>
@@ -11363,7 +11373,7 @@
       </c>
       <c r="K278" s="24"/>
     </row>
-    <row r="279" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A279" s="24" t="s">
         <v>106</v>
       </c>
@@ -11392,7 +11402,7 @@
       </c>
       <c r="K279" s="24"/>
     </row>
-    <row r="280" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A280" s="24" t="s">
         <v>38</v>
       </c>
@@ -11423,7 +11433,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="281" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A281" s="24" t="s">
         <v>570</v>
       </c>
@@ -11452,7 +11462,7 @@
       </c>
       <c r="K281" s="24"/>
     </row>
-    <row r="282" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A282" s="24" t="s">
         <v>569</v>
       </c>
@@ -11481,7 +11491,7 @@
       </c>
       <c r="K282" s="24"/>
     </row>
-    <row r="283" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A283" s="24" t="s">
         <v>547</v>
       </c>
@@ -11510,7 +11520,7 @@
       </c>
       <c r="K283" s="24"/>
     </row>
-    <row r="284" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A284" s="24" t="s">
         <v>578</v>
       </c>
@@ -11539,7 +11549,7 @@
       </c>
       <c r="K284" s="24"/>
     </row>
-    <row r="285" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A285" s="12" t="s">
         <v>868</v>
       </c>
@@ -11564,7 +11574,7 @@
       </c>
       <c r="K285" s="28"/>
     </row>
-    <row r="286" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A286" s="12" t="s">
         <v>869</v>
       </c>
@@ -11589,7 +11599,7 @@
       </c>
       <c r="K286" s="28"/>
     </row>
-    <row r="287" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A287" s="24" t="s">
         <v>575</v>
       </c>
@@ -11618,135 +11628,135 @@
       </c>
       <c r="K287" s="24"/>
     </row>
-    <row r="288" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A288" s="12" t="s">
+        <v>916</v>
+      </c>
+      <c r="B288" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C288" s="32" t="s">
+        <v>917</v>
+      </c>
+      <c r="D288" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="E288" s="12" t="s">
+        <v>918</v>
+      </c>
+      <c r="F288" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G288" s="28"/>
+      <c r="H288" s="28"/>
+      <c r="I288" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J288" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K288" s="28"/>
+    </row>
+    <row r="289" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A289" s="12" t="s">
         <v>716</v>
       </c>
-      <c r="B288" s="12" t="s">
+      <c r="B289" s="12" t="s">
         <v>847</v>
       </c>
-      <c r="C288" s="12" t="s">
+      <c r="C289" s="12" t="s">
         <v>717</v>
       </c>
-      <c r="D288" s="12"/>
-      <c r="E288" s="12" t="s">
+      <c r="D289" s="12"/>
+      <c r="E289" s="12" t="s">
         <v>718</v>
       </c>
-      <c r="F288" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G288" s="13"/>
-      <c r="H288" s="13"/>
-      <c r="I288" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J288" s="13" t="s">
+      <c r="F289" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G289" s="13"/>
+      <c r="H289" s="13"/>
+      <c r="I289" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J289" s="13" t="s">
         <v>752</v>
       </c>
-      <c r="K288" s="12"/>
-    </row>
-    <row r="289" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A289" s="12" t="s">
+      <c r="K289" s="12"/>
+    </row>
+    <row r="290" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A290" s="12" t="s">
         <v>673</v>
-      </c>
-      <c r="B289" s="12" t="s">
-        <v>856</v>
-      </c>
-      <c r="C289" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="D289" s="20" t="s">
-        <v>740</v>
-      </c>
-      <c r="E289" s="12" t="s">
-        <v>803</v>
-      </c>
-      <c r="F289" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G289" s="12"/>
-      <c r="H289" s="12"/>
-      <c r="I289" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J289" s="12" t="s">
-        <v>543</v>
-      </c>
-      <c r="K289" s="12"/>
-    </row>
-    <row r="290" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A290" s="12" t="s">
-        <v>742</v>
       </c>
       <c r="B290" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C290" s="20" t="s">
-        <v>743</v>
-      </c>
-      <c r="D290" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="D290" s="20" t="s">
         <v>740</v>
       </c>
       <c r="E290" s="12" t="s">
-        <v>744</v>
-      </c>
-      <c r="F290" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="G290" s="13"/>
-      <c r="H290" s="13"/>
-      <c r="I290" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="J290" s="13" t="s">
+        <v>803</v>
+      </c>
+      <c r="F290" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G290" s="12"/>
+      <c r="H290" s="12"/>
+      <c r="I290" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J290" s="12" t="s">
         <v>543</v>
       </c>
       <c r="K290" s="12"/>
     </row>
-    <row r="291" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A291" s="12" t="s">
         <v>742</v>
       </c>
       <c r="B291" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C291" s="12" t="s">
+      <c r="C291" s="20" t="s">
         <v>743</v>
       </c>
       <c r="D291" s="12" t="s">
         <v>740</v>
       </c>
       <c r="E291" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="F291" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G291" s="13"/>
+      <c r="H291" s="13"/>
+      <c r="I291" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="J291" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="K291" s="12"/>
+    </row>
+    <row r="292" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A292" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="B292" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C292" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="D292" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="E292" s="12" t="s">
         <v>745</v>
-      </c>
-      <c r="F291" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G291" s="12"/>
-      <c r="H291" s="12"/>
-      <c r="I291" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J291" s="12" t="s">
-        <v>543</v>
-      </c>
-      <c r="K291" s="12"/>
-    </row>
-    <row r="292" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A292" s="12" t="s">
-        <v>757</v>
-      </c>
-      <c r="B292" s="12" t="s">
-        <v>848</v>
-      </c>
-      <c r="C292" s="12" t="s">
-        <v>758</v>
-      </c>
-      <c r="D292" s="12" t="s">
-        <v>723</v>
-      </c>
-      <c r="E292" s="12" t="s">
-        <v>759</v>
       </c>
       <c r="F292" s="12" t="s">
         <v>497</v>
@@ -11757,40 +11767,69 @@
         <v>517</v>
       </c>
       <c r="J292" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K292" s="12"/>
+    </row>
+    <row r="293" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A293" s="12" t="s">
+        <v>757</v>
+      </c>
+      <c r="B293" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="C293" s="12" t="s">
+        <v>758</v>
+      </c>
+      <c r="D293" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="E293" s="12" t="s">
+        <v>759</v>
+      </c>
+      <c r="F293" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G293" s="12"/>
+      <c r="H293" s="12"/>
+      <c r="I293" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J293" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="K292" s="12"/>
-    </row>
-    <row r="293" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A293" s="28" t="s">
+      <c r="K293" s="12"/>
+    </row>
+    <row r="294" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A294" s="28" t="s">
         <v>901</v>
       </c>
-      <c r="B293" s="12" t="s">
+      <c r="B294" s="12" t="s">
         <v>902</v>
       </c>
-      <c r="C293" s="12" t="s">
+      <c r="C294" s="12" t="s">
         <v>903</v>
       </c>
-      <c r="D293" s="28"/>
-      <c r="E293" s="12" t="s">
+      <c r="D294" s="28"/>
+      <c r="E294" s="12" t="s">
         <v>904</v>
       </c>
-      <c r="F293" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="G293" s="28"/>
-      <c r="H293" s="28"/>
-      <c r="I293" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="J293" s="12" t="s">
+      <c r="F294" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="G294" s="28"/>
+      <c r="H294" s="28"/>
+      <c r="I294" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="J294" s="12" t="s">
         <v>905</v>
       </c>
-      <c r="K293" s="28"/>
+      <c r="K294" s="28"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G412">
-    <sortCondition ref="A1:A412"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G413">
+    <sortCondition ref="A1:A413"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>